<commit_message>
Add all location from Wroclaw. Lable pins with commision number.
</commit_message>
<xml_diff>
--- a/location.xlsx
+++ b/location.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\komisjaFinder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31C30BC5-4755-4B89-AFF7-883BF9DAAD73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97AE4E3D-A3E6-46F1-B6B3-0E958ACF0C78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="994" uniqueCount="529">
   <si>
     <t>number</t>
   </si>
@@ -529,6 +529,1089 @@
   </si>
   <si>
     <t>address</t>
+  </si>
+  <si>
+    <t>Wrocław-Krzyki ulice: Gajowicka 62 - 88 parzyste, Zaporoska 42 - 62 parzyste, 49 - 51 nieparzyste</t>
+  </si>
+  <si>
+    <t>Szkoła Podstawowa nr 76 z Oddziałami Sportowymi, ul. Wandy 13, 53-320 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Krzyki ulice: Gajowicka 122 - 148 parzyste, al. gen. Józefa Hallera 3 - 29A nieparzyste, Krakusa, Podchorążych, Słowicza, Spadochroniarzy, Sztabowa 28 - 66 parzyste, 51 - 83 nieparzyste, Wandy</t>
+  </si>
+  <si>
+    <t>Wrocław-Krzyki ulice: Pocztowa, Powstańców Śląskich 121 - 143 nieparzyste, 128 - 154 parzyste, Sztabowa 72 - 100A parzyste, 85 - 107 nieparzyste, Ślężna 115-129, 129A, al. Wiśniowa 4 - 36D parzyste, 70</t>
+  </si>
+  <si>
+    <t>Szkoła Podstawowa nr 81, ul. Jastrzębia 26, 53-148 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Krzyki ulice: Bolesława Ulanowskiego, Gajowicka 154 - 174 parzyste, 188 - 200 parzyste, al. gen. Józefa Hallera 2 - 34 parzyste, Jastrzębia, Sokola 18 - 32 parzyste, 27 - 51 nieparzyste</t>
+  </si>
+  <si>
+    <t>Szkoła Podstawowa Nr 81, ul. Jastrzębia 26, 53-148 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Krzyki ulice: Orla, Powstańców Śląskich 145, 159 - 219 nieparzyste, 160 - 182A parzyste, Racławicka 1 - 36/38, Sępia, Wolbromska</t>
+  </si>
+  <si>
+    <t>Wrocław-Krzyki ulice: al. gen. Józefa Hallera 36 - 48 parzyste, 52, Racławicka 37 - 62A, Wrocław-Fabryczna ulice: Gajowicka 175 - 199 nieparzyste, Modlińska, pl. Mordechaja Anielewicza, Oksywska, Przelot, Saperów, Sokola 5 - 23A nieparzyste, 6 - 14 parzyste, Żurawia</t>
+  </si>
+  <si>
+    <t>Szkoła Podstawowa nr 4, ul. Powstańców Śląskich 210 - 218, 53-140 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Krzyki ulice: Andrzeja Waligórskiego, Jana Kaczmarka, Januszowicka, Kampinoska, Powstańców Śląskich 186 - 222 parzyste, Pułtuska, Sochaczewska, Sokola 52 - 79, Ślężna 197 - 227</t>
+  </si>
+  <si>
+    <t>Liceum Ogólnokształcące nr V, ul. Jacka Kuronia 14, 50-550 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Krzyki ulice: al. Armii Krajowej 1, Cisowa, Garwolińska, Grójecka, Kutnowska, Rawska, Rudolfa Weigla, Skierniewicka, Ślężna 88 - 128A parzyste, 130 - 196, Wiktora Brossa, al. Wiśniowa 1 - 87 nieparzyste</t>
+  </si>
+  <si>
+    <t>Zespół Szkolno-Przedszkolny nr 19, ul. Januszowicka 35 - 37, 53-135 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Krzyki ulice: al. Akacjowa, al. Dębowa, al. Jarzębinowa, al. Jaworowa, al. Kasztanowa, al. Lipowa, Sudecka 98 - 120 parzyste, 122 - 166, al. Wiązowa</t>
+  </si>
+  <si>
+    <t>Ośrodek Postaw Twórczych Zamek, ul. Działkowa 15, 50-538 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Krzyki ulice: Czerniawska, Dusznicka, Działkowa, Kudowska, Lądecka, Niemczańska, Puszczykowska, Strońska, Świeradowska 1 - 37</t>
+  </si>
+  <si>
+    <t>Zespół Szkolno-Przedszkolny nr 21, ul. Kłodzka 40, 50-536 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Krzyki ulice: Alpejska, Bogusława Bobrańskiego, Borowska 134 - 272 parzyste, 177 - 283B nieparzyste, Długopolska, Himalajska, Pamirska, Pirenejska, Wandy Rutkiewicz</t>
+  </si>
+  <si>
+    <t>Zespół Szkół nr 2, ul. Borowska 105, 50-551 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Krzyki ulice: al. Armii Krajowej 5, 37, 41, Brzoskwiniowa, Jabłeczna, Spiska 52 - 64A, Żegiestowska</t>
+  </si>
+  <si>
+    <t>Szkoła Podstawowa nr 90, ul. Orzechowa 62, 50-540 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Krzyki ulice: gen. Mariusza Zaruskiego, Krynicka 7 - 51 nieparzyste, 84 - 92 parzyste, Mieczysława Orłowicza, Romana Zmorskiego, Zygmunta Glogera</t>
+  </si>
+  <si>
+    <t>Wrocław-Krzyki ulice: Bardzka 3 - 5 nieparzyste, Krynicka 2 - 82 parzyste, Świeradowska 67 - 77</t>
+  </si>
+  <si>
+    <t>Wrocław-Krzyki ulice: Bielawska, Dzierżoniowska, Pieszycka, Pietrzykowicka, Piławska, Radkowska, Świeradowska 41 - 65 nieparzyste, Wambierzycka</t>
+  </si>
+  <si>
+    <t>Wrocław-Krzyki ulica Orzechowa 44 - 62A, 91 - 114</t>
+  </si>
+  <si>
+    <t>Wrocław-Krzyki ulica Orzechowa 2 - 43</t>
+  </si>
+  <si>
+    <t>Dzienny Dom Pomocy Społecznej "Na Ciepłej", ul. Ciepła 15b, 50-524 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Krzyki ulice: Ciepła, Marka Petrusewicza, Sieradzka, Wesoła</t>
+  </si>
+  <si>
+    <t>Szkoła Podstawowa nr 73, ul. Gliniana 30, 50-525 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Krzyki ulice: Borowska 9, 6 - 52 parzyste, Gliniana 2 - 38, 39 - 69 nieparzyste, Łódzka 6 - 14 parzyste, 1 - 19 nieparzyste, Ślężna 2 - 28 parzyste</t>
+  </si>
+  <si>
+    <t>Zespół Szkół Logistycznych, ul. Jana Władysława Dawida 9 - 11, 50-527 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Krzyki ulice: Dyrekcyjna, Gajowa 21 - 43 nieparzyste, 28 - 68A parzyste, Gliniana 40 - 60 parzyste, 71 - 89 nieparzyste, Jana Władysława Dawida, Joannitów, Sucha</t>
+  </si>
+  <si>
+    <t>Zespół Szkół Gastronomicznych, ul. Kamienna 86, 50-547 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Krzyki ulice: Borowska 74, Gajowa 47 - 55 nieparzyste, Przestrzenna 1 - 29, 32 - 36 parzyste, Tomaszowska</t>
+  </si>
+  <si>
+    <t>Zespół Szkolno-Przedszkolny nr 17, ul. Wieczysta 105, 50-550 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Krzyki ulice: Gajowa 70 - 80 parzyste, Kamienna 74 - 154, Łódzka 16 - 46A parzyste, 23 - 47 nieparzyste, pl. Ludwika Zamenhofa, Ślężna 78 - 86 parzyste</t>
+  </si>
+  <si>
+    <t>Wrocław-Krzyki ulice: Boczna, Gajowa 1 - 19 nieparzyste, 8 - 26 parzyste, Gliniana 89A - 99 nieparzyste, 62 - 68 parzyste, Hubska 1 - 5, 7 - 69, Lniana</t>
+  </si>
+  <si>
+    <t>Szkoła Podstawowa nr 77, ul. św. Jerzego 4, 50-518 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Krzyki ulice: Hubska 70 - 123A, Jesionowa 2 - 14 parzyste, Paczkowska 3, Prudnicka 1 - 11 nieparzyste, 2 - 12A parzyste, Przestrzenna 38 - 50 parzyste, św. Jerzego, Wapienna</t>
+  </si>
+  <si>
+    <t>Wrocław-Krzyki ulice: al. Armii Krajowej 2 - 40 parzyste, 50, Bardzka 1, 1A, 1C, Przestrzenna 31 - 49 nieparzyste, Śliczna 54 - 66 parzyste, Widna, Wieczysta 151 - 175 nieparzyste</t>
+  </si>
+  <si>
+    <t>Wrocław-Krzyki ulice: Borowska 86 - 118 parzyste, 101 - 145 nieparzyste, Jacka Kuronia, Spiska 1, Śliczna 1 - 38</t>
+  </si>
+  <si>
+    <t>Wrocław-Krzyki ulice: Śliczna 39 - 44B, 45 - 59 nieparzyste, Wieczysta 63 - 149 nieparzyste</t>
+  </si>
+  <si>
+    <t>Szkoła Podstawowa nr 9, ul. Nyska 66, 50-505 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Krzyki ulice: Henrykowska, Hubska 6, Nyska</t>
+  </si>
+  <si>
+    <t>Wrocław-Krzyki ulice: Bardzka 2 - 30 parzyste, 60, 80, Jesionowa 9 - 49 nieparzyste, 16 - 78 parzyste, Otmuchowska, Paczkowska 26-50 parzyste, Sernicka</t>
+  </si>
+  <si>
+    <t>PGNiG Obrót Detaliczny sp. z o. o. Region Dolnośląski-budynek G, ul. Gazowa 3, 50-513 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Krzyki ulice: al. Armii Krajowej 45 - 61 nieparzyste, 46 - 48S parzyste, 54, 62, bp. Bernarda Bogedaina, Gazowa, Kamieniecka, ks. Czesława Klimasa, Laskowa, Łagiewnicka, Międzyleska, Morelowa, Morwowa, Owocowa, Śliwkowa, Tarnogajska, Winogronowa, Ząbkowicka, Ziębicka, Złotostocka</t>
+  </si>
+  <si>
+    <t>Szkoła Podstawowa Nr 96, ul. Krakowska 2, 50-425 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Krzyki ulice: Bierdzańska 3, 4 - 12 parzyste, gen. Romualda Traugutta 135 - 149 nieparzyste, 132 - 146 parzyste, Krakowska 1 - 105 nieparzyste, 2 - 128 parzyste, Krzywa Grobla, Międzyrzecka, Młoda, Na Grobli, Na Niskich Łąkach, Nizinna, Okólna, Opatowicka 1, Rakowiecka, Stanisława Więckowskiego 1 - 16, Wilcza, Żabia Grobla, Żabia Ścieżka</t>
+  </si>
+  <si>
+    <t>Wrocław-Krzyki ulice: gen. Romualda Traugutta 80 - 130 parzyste, 93 - 133A nieparzyste, 133OF, Zgodna, pl. Zgody</t>
+  </si>
+  <si>
+    <t>Liceum Ogólnokształcące nr IV, ul. Stacha Świstackiego 12 - 14, 50-430 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Krzyki ulice: Brzeska, gen. Ignacego Prądzyńskiego 26 - 54 parzyste, 45 - 63 nieparzyste, Stanisława Chudoby, Stanisława Więckowskiego 19 - 37</t>
+  </si>
+  <si>
+    <t>Wrocław-Krzyki ulice: Komuny Paryskiej 79 - 85 nieparzyste, 82 - 96 parzyste, Stacha Świstackiego, Tadeusza Kościuszki 152 do końca parzyste, 159 do końca nieparzyste</t>
+  </si>
+  <si>
+    <t>Zespół Szkół Teleinformatycznych i Elektronicznych (Budynek Hali Sportowej), ul. Stanisława Worcella 20 - 26, 50-448 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Krzyki ulice: gen. Ignacego Prądzyńskiego 1A - 11 nieparzyste, 29 - 43 nieparzyste, gen. Kazimierza Pułaskiego 4 - 56 parzyste, 47 - 49A nieparzyste, Komuny Paryskiej 43 - 73A nieparzyste, Tadeusza Kościuszki 108 - 150 parzyste, 109 - 149 nieparzyste</t>
+  </si>
+  <si>
+    <t>Muzeum Etnograficzne, ul. gen. Romualda Traugutta 111/113, 50-419 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Krzyki ulice: gen. Romualda Traugutta 57/59, 61 - 91 nieparzyste, 52 - 78 parzyste, Miernicza 2 - 16, Szybka, Waleriana Łukasińskiego</t>
+  </si>
+  <si>
+    <t>Szkoła Podstawowa nr 2, ul. Komuny Paryskiej 36 - 38, 50-451 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Krzyki ulice: Dworcowa 22 - 32 parzyste, gen. Antoniego Madalińskiego, gen. Jana Henryka Dąbrowskiego 26 - 50 parzyste, gen. Kazimierza Pułaskiego 67 - 81 nieparzyste, pl. Konstytucji 3 Maja, Stanisława Małachowskiego, Tadeusza Kościuszki 72 - 106 parzyste, 77 - 107 nieparzyste</t>
+  </si>
+  <si>
+    <t>Szermiercza Sportowa Szkoła Podstawowa nr 85, ul. gen. Romualda Traugutta 37, 50-416 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Krzyki ulice: Dobrzyńska, gen. Józefa Haukego-Bosaka 1 - 10, gen. Romualda Traugutta 1 - 45, 55, pl. gen. Walerego Wróblewskiego, wyb. Juliusza Słowackiego, Kujawska, Mazowiecka, Podwale 73 - 83 nieparzyste, 74 - 84 parzyste, Walońska, Zygmunta Krasińskiego, Wrocław-Stare Miasto pl. Powstańców Warszawy 1</t>
+  </si>
+  <si>
+    <t>Liceum Ogólnokształcące nr XIII, ul. gen. Józefa Haukego-Bosaka 33 - 37, 50-447 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Krzyki ulice: gen. Ignacego Prądzyńskiego 4 - 24A parzyste, 13 - 25 nieparzyste, gen. Karola Kniaziewicza 15 - 40, Komuny Paryskiej 48 - 78 parzyste, Miernicza 17 - 28</t>
+  </si>
+  <si>
+    <t>Zespół Szkół Teleinformatycznych i Elektronicznych, ul. gen. Józefa Haukego-Bosaka 21, 50-447 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Krzyki ulice: gen. Józefa Haukego-Bosaka 11 - 37, gen. Karola Kniaziewicza 1 - 14, Stanisława Worcella</t>
+  </si>
+  <si>
+    <t>Zespół Szkół Ekonomiczno-Administracyjnych, ul. Stanisława Worcella 3, 50-448 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Krzyki ulice: Aleksandra Hercena, Dworcowa 2 - 20 parzyste, gen. Henryka Dąbrowskiego 1 - 18, 19 - 37A nieparzyste, Komuny Paryskiej 3 - 41, 42 - 46 parzyste, Podwale 67 - 71 nieparzyste, 68 - 72 parzyste</t>
+  </si>
+  <si>
+    <t>Siedziba Rady Osiedla Księże, ul. Rybnicka 39-41, 52-016 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Krzyki ulice: Blizanowicka, Cieszyńska, Czechowicka, Księska, Opatowicka 10 - 156 parzyste, 11 - 145 nieparzyste, Pszczyńska, Rybnicka, Siemianowicka, Starodworska, Świątnicka, Wadowicka, Wodzisławska, Zabrzańska, Zagłębiowska, Zalewowa, Zawierciańska</t>
+  </si>
+  <si>
+    <t>Szkoła Podstawowa nr 99, ul. Głubczycka 3, 52-024 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Krzyki ulice: Brochowska 3 - 23 nieparzyste, 4 - 22 parzyste, Chorzowska, Gliwicka, Głubczycka, Górnośląska, Hajducka, Karola Skibińskiego, Karwińska, Katowicka, Kozielska, Krakowska 119 - 149 nieparzyste, 148 - 182 parzyste, Opolska 100 - 197, Raciborska, Tarnogórska</t>
+  </si>
+  <si>
+    <t>Brochowskie Centrum Aktywności Lokalnej we Wrocławiu, ul. Koreańska 1a, 52-121 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Krzyki ulice: Arabska, Boiskowa, Cedrowa, Ignacego Mościckiego 47 - 51, Jana Wesołowskiego, Japońska, Jemeńska, Jordańska, Leonarda da Vinci, Lisia, Marsowa, Opolska 199, Palestyńska, Pięćdziesięciu Bohaterów, Pionierów, Sadowa, Syjamska, Topolowa, Warszawska, Węgierska, Wiaduktowa, Wietnamska, Wileńska, Ziemniaczana</t>
+  </si>
+  <si>
+    <t>Szkoła Podstawowa nr 80, ul. Polna 4, 52-120 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Krzyki ulice: Afgańska, Armeńska, Bengalska, Bluszczowa, Chmurna, Cypryjska, Filipińska, Gruzińska, Ignacego Mościckiego 1 - 45 nieparzyste, 2 - 46 parzyste, 99 - 111 nieparzyste, 102 - 112 parzyste, Indonezyjska, pl. Indyjski, Iracka, Koreańska, Libańska, Malezyjska, Mandżurska, Nepalska, Pakistańska, Perska, Piwniczna, al. Róż, Społeczna, Syryjska, Tadżycka, Tajwańska, Tybetańska, Uzbecka, Woskowa</t>
+  </si>
+  <si>
+    <t>Wrocław-Krzyki ulice: 3 Maja, Biegła, Birmańska, Centralna, Chińska, Kazachstańska, Krótka, Laotańska, pl. Mongolski, Polna, Semaforowa, Tatarska</t>
+  </si>
+  <si>
+    <t>Miejska Biblioteka Publiczna Filia nr 14 Centrum Aktywności Lokalnej Dobre Czasy na Jagodnie, ul. Sygnałowa 23, 52-130 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Krzyki ulice: Braci Hofmannów, Buforowa 2-72B parzyste, Drezynowa, Ekspresowa, Ernesta Malinowskiego, Godfryda Linkego, Hipolita Cegielskiego, Konduktorska, Lokomotywowa, Maszynistów, Nastawnicza, Parowozowa, Rozjazdowa, Rudolfa Modrzejewskiego, Sygnałowa, Szynowa, Trakcyjna, Tunelowa, Wilhelma Grapowa, Zwrotnicza</t>
+  </si>
+  <si>
+    <t>Rada Osiedla Jagodno, ul. Jagodzińska 15, 52-129 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Krzyki ulice: Brzozowa, Buforowa 69-91A nieparzyste, Beli Bartoka, Dróżnicza, Franza Petera Schuberta 4-24a parzyste, Igora Strawińskiego, Jagodzińska, Johanna Straussa, Johannesa Brahmsa, Ludwiga van Beethovena, Maurycego Ravela, Ryszarda Wagnera</t>
+  </si>
+  <si>
+    <t>Świetlica "Cztery Pory Roku-Zima", ul. Ryszarda Wagnera 3, 52-129 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Krzyki ulice: Antonia Vivaldiego, Buforowa 97-121C nieparzyste, 100-112 parzyste, Franza Petera Schuberta 26-76 parzyste</t>
+  </si>
+  <si>
+    <t>Szkoła Podstawowa nr 23, ul. Przystankowa 32, 52-231 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Krzyki ulice: Antoniego Czechowa, Asfaltowa, Będzińska, Bliska, Daleka, Glebowa, Granitowa, Kosmiczna, Marmurowa, Nenufarowa, Oraczy, Pachnąca, Parafialna 1 - 59 nieparzyste, 2 - 30 parzyste, Pawia, Pawła Jasienicy, Przystankowa, Radarowa, Radłowa, Ratajów, Rozmarynowa, Siewców, Snopkowa, Spokojna, Szarych Szeregów, Świt 26 - 94 parzyste, Terenowa, Wylotowa, Żeńców, Żniwna</t>
+  </si>
+  <si>
+    <t>Wrocław-Krzyki ulice: Jana Lechonia, Jarosława Iwaszkiewicza, Kazimiery Iłłakowiczówny, Kazimierza Wierzyńskiego, Konstantego Ildefonsa Gałczyńskiego 27 - 45 nieparzyste, 36 - 46 parzyste, Mirona Białoszewskiego, Oboźna, Smardzowska, Wisławy Szymborskiej</t>
+  </si>
+  <si>
+    <t>Wrocław-Krzyki ulice: Andrzeja Małkowskiego, Biwakowa, Chlebowa, gen. Stefana Grota-Roweckiego 2 - 190 parzyste, 13 - 109 nieparzyste, Gerberowa 1 - 7 nieparzyste, Hufcowa, Klasztorna, Kwitnąca, Olgi Drahonowskiej, Poronińska, Skibowa, Tulipanowa 3 - 43 nieparzyste, Wspólna 7 - 13 nieparzyste, Zastępowa, Zawiszy Czarnego, Zuchowa</t>
+  </si>
+  <si>
+    <t>Zespół Szkolno-Przedszkolny nr 6, ul. Konstantego Ildefonsa Gałczyńskiego 8, 52-214 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Krzyki ulice: Agrestowa 98B - 128 parzyste, 142, Bartłomieja Strachowskiego, gen. Franciszka Kleeberga, gen. Franciszka Włada, gen. Józefa Kustronia, gen. Juliana Filipowicza, gen. Marii Wittek, gen. Mikołaja Bołtucia, gen. Stanisława Grzmota-Skotnickiego, Łubinowa, marsz. Edwarda Rydza-Śmigłego, mjr. Henryka Sucharskiego, Motylkowa, Nektarowa, Obrońców Poczty Gdańskiej 10 - 114 parzyste, 134 - 138 parzyste, Orawska, Pigwowa, Pistacjowa, płk. Kazimierza Masztalerza, płk. Stanisława Dąbka, Pszczelarska, Rzepakowa, Sojowa, Stefana Starzyńskiego, Świt 65 - 97 nieparzyste, Ułańska</t>
+  </si>
+  <si>
+    <t>Wrocław-Krzyki ulice: adm. Józefa Unruga, Czołgistów, Fizylierska, gen. Kazimierza Sosnkowskiego, gen. Romana Abrahama, gen. Tadeusza Kutrzeby, Marcelego Nenckiego, mjr. Hubala, Parafialna 32 - 70 parzyste, 61 - 79 nieparzyste, Piechoty, Synów Pułku, Szczepowa, Uczniowska, Zwiadowców</t>
+  </si>
+  <si>
+    <t>Wrocław-Krzyki ulice: Agatowa, Ametystowa, Brylantowa, Bursztynowa, Diamentowa, gen. Grota-Roweckiego 111 - 209 nieparzyste, Gerberowa 2 - 22 parzyste, Jarzynowa, Jaspisowa, Konstantego Ildefonsa Gałczyńskiego 1 - 25 nieparzyste, 4 - 32 parzyste, Kontradmirała Stefana Frankowskiego, Koralowa, Kryniczna, Kryształowa, Kurpiów, Malachitowa, Nefrytowa, Opalowa, Rubinowa, Storczykowa, Strączkowa, Szmaragdowa, Traktorowa, Turkusowa, Walerego Goetla, Władysława Szafera, Zdrojowa</t>
+  </si>
+  <si>
+    <t>Zespół Szkolno-Przedszkolny nr 16, ul. Wietrzna 50, 53-024 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Krzyki ulice: Jesienna, Krzycka 1 - 86H, Letnia, Polarna, Przyjaźni 39 - 141A nieparzyste, Wiosenna, Zimowa</t>
+  </si>
+  <si>
+    <t>Szkoła Podstawowa nr 64, ul. Wojszycka 1, 53-006 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Krzyki ulice: Agrestowa 2 - 66 parzyste, 1 - 93 nieparzyste, Aliancka, Borówczana, Czeremchowa, Czereśniowa, Dereniowa, Hippiczna, Kalinowa, Kolarska, Końska, Koszycka, Malinowa, Okrężna, Ołtaszyńska, Ożynowa, Porzeczkowa, Stajenna, Tarninowa, Tenisowa, Turniejowa, Warsztatowa, Wojszycka, Wyścigowa, Zapaśnicza, Żołnierska</t>
+  </si>
+  <si>
+    <t>Wrocław-Krzyki ulice: Agrestowa 101 - 145 nieparzyste, gen. Stanisława Maczka, Husarska, Jagodowa, Kawalerzystów, Obrońców Poczty Gdańskiej 1 - 19A nieparzyste, Poziomkowa, Szwoleżerska, Truskawkowa</t>
+  </si>
+  <si>
+    <t>Wrocław-Krzyki ulice: Burzowa, Gradowa, Południowa, Poranna, Powiewna, Wichrowa, Wieczorna, Wietrzna 26 - 46 parzyste, 109A - 137 nieparzyste, Zefirowa</t>
+  </si>
+  <si>
+    <t>Szkoła Podstawowa nr 61, ul. Skarbowców 8, 53-025 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Krzyki ulice: Chłodna, Deszczowa, Halna, Juliana Tuwima, ks. Piotra Wawrzyniaka, Mariana Rapackiego, Pogodna, Skarbowców 4 - 87A, Słotna, Sowia, Stanisława Kusztelana, Szronowa, Upalna, Wietrzna 2 - 24 parzyste, 3 - 107 nieparzyste, Wojciecha Korfantego</t>
+  </si>
+  <si>
+    <t>Wrocław-Krzyki ulice: Babiego Lata, Krzycka 87 - 107, Mglista, Róży Wiatrów, Skarbowców 89 - 123, Skrajna, Szarugi, Życzliwa</t>
+  </si>
+  <si>
+    <t>Wrocław-Krzyki ulice: Braterska, al. Karkonoska 7 - 65 nieparzyste, 8 - 54 parzyste, Przyjaźni 2 - 66 parzyste, Rodzinna, Sąsiedzka, Siostrzana</t>
+  </si>
+  <si>
+    <t>Szkoła Podstawowa nr 42, ul. Wałbrzyska 50, 52-314 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Krzyki ulice: Balladyny, Chyżan, Cukrozetka, Czekoladowa, Dalemińców, Goleszan, Goplan, al. Karkonoska 83, 83A, Karmelkowa 51 - 59 nieparzyste, 70 - 74 parzyste, 81 - 89 nieparzyste, 82 - 94 parzyste, Łuczan, Łysogórska, Marcepanowa, Piernikowa, Połabian, Przemysłowa, Redarów, Sezamkowa, Siedliczan, Słoneczna, Słowińców, Waflowa, Wałbrzyska 1 - 14, Wolinian, Zabrodzka</t>
+  </si>
+  <si>
+    <t>Wrocław-Krzyki ulice: Buraczana, Dożynkowa, Jutrzenki 2 - 70A parzyste, 5 - 47 nieparzyste, Kabaczkowa, Kostrzyńska, Marchewkowa, Ogórkowa, Szparagowa</t>
+  </si>
+  <si>
+    <t>Wrocław-Krzyki ulice: Cukrowa, Józefa Supińskiego, Kobierzycka, Kościelna, Łanowa, Międzygórska, Migdałowa, Wałbrzyska 15 - 61H</t>
+  </si>
+  <si>
+    <t>Zespół Szkolno-Przedszkolny nr 9, ul. Ludwika Solskiego 13, 52-401 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Fabryczna ulice: Fryderyka Skarbka, Harcerska, Jordanowska, Karmelkowa 2 - 50 parzyste, 5 - 35 nieparzyste, 41, Karola Darwina, ks. Jana Dzierżonia, Ludwika Solskiego, Marcina Bukowskiego 1 - 49A, Michała Śniegockiego, Mokronoska, al. Piastów 1 - 29, Stanisława Pękalskiego, Stanisława Rosponda, Tadeusza Mikulskiego, Turystyczna, Wiejska, Władysława Chachaja</t>
+  </si>
+  <si>
+    <t>Wrocław-Fabryczna ulice: Cesarzowicka, Emila Zoli, Eugeniusza Kwiatkowskiego 2 - 12 parzyste, 3 - 15 nieparzyste, Honoriusza Balzaka, Ibn Siny Awicenny 21 - 23 nieparzyste, 30 - 54 parzyste, 45 - 53 nieparzyste, Karola Adamieckiego, Leona Petrażyckiego, Leszczynowa, Tadeusza Wendy, Tyniecka</t>
+  </si>
+  <si>
+    <t>Zespół Szkolno-Przedszkolny nr 9, ul. Mariana Morelowskiego 43, 52-429 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Fabryczna ulice: Anioła Ślązaka, bł. Wincentego Kadłubka, Bronisława Trentowskiego, Ewy i Karola Maleczyńskich, Giełdowa, Hugona Steinhausa, Jana Nikliborca, Jana Ostroroga, Jana Stanki, Jerzego Kowalskiego, Jutrzenki 59 - 61 nieparzyste, 71 - 85 nieparzyste, 74 - 110 parzyste, Kamila Stefki, Karmelkowa 52 - 66 parzyste, 65A, ks. Hieronima Feichta, Kupiecka, Marcina Bukowskiego 50 - 180, Mariana Morelowskiego, Mariana Suskiego, al. Piastów 30 - 99, Seweryna Wysłoucha, Sobótki, Witolda Taszyckiego, Zofii Nałkowskiej, Wrocław-Krzyki ulica Targowa</t>
+  </si>
+  <si>
+    <t>Sportowa Szkoła Podstawowa nr 46, ul. Ścinawska 21, 53-628 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Stare Miasto ulice: Długa, Gnieźnieńska, Inowrocławska 48 - 56 parzyste, 63 - 65, Kazimierza Michalczyka, Łęczycka, Młodych Techników 17, 47 - 66, Portowa, Poznańska 29 - 37 nieparzyste, 48-80, 58, Salezjańska, Sołtysia, Starogroblowa</t>
+  </si>
+  <si>
+    <t>Wrocław-Stare Miasto ulice: Głogowska 13 - 35 nieparzyste, Lubińska 36 - 54, Poznańska 15 - 25 nieparzyste, Rynek Szczepiński, Zielonogórska</t>
+  </si>
+  <si>
+    <t>Wrocław-Stare Miasto ulice: Chojnowska, Głogowska 14 - 30 parzyste, 37 - 53 nieparzyste, Głośna, Słubicka, Szprotawska, Zgorzelecka, Żagańska, Wrocław-Fabryczna ulica Przedmiejska</t>
+  </si>
+  <si>
+    <t>Wrocławski Zakład Aktywności Zawodowej, ul. Litomska 10, 53-641 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Stare Miasto ulice: Ścinawska, Zachodnia 1 - 55 nieparzyste, 8 - 10 parzyste</t>
+  </si>
+  <si>
+    <t>Wrocław-Stare Miasto ulice: Kruszwicka 5 - 31 nieparzyste, 6, 6A, 8, 8A, Litomska 3 - 9 nieparzyste, 17 - 29 nieparzyste, Stefana Czarnieckiego 2 - 28 parzyste, 1 - 9 nieparzyste</t>
+  </si>
+  <si>
+    <t>Zespół Szkolno-Przedszkolny nr 18, ul. Poznańska 26, 53-630 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Stare Miasto ulice: Głogowska 1 - 11, Legnicka 33 - 33D, Poznańska 14 - 26 parzyste, Zachodnia 26 - 44 parzyste, 50, 52</t>
+  </si>
+  <si>
+    <t>Elektroniczne Zakłady Naukowe, ul. Braniborska 57, 53-680 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Stare Miasto ulice: Bolesławiecka, Legnicka 39, 43 - 48, Stacyjna, Strzegomska 3 - 9 nieparzyste, 2 - 12 parzyste, 36 - 42N parzyste, 47 - 57 nieparzyste, pl. Strzegomski, Śrubowa, św. Pawła, Złotoryjska, Wrocław-Fabryczna ulice: Bolkowska, Jaworska</t>
+  </si>
+  <si>
+    <t>Wrocław-Stare Miasto ulice: Lubińska 1 - 30, 83, Stefana Czarnieckiego 13 - 41 nieparzyste, 52 - 80 parzyste</t>
+  </si>
+  <si>
+    <t>Szkoła Podstawowa nr 14, ul. Zachodnia 2, 53-644 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Stare Miasto ulice: Kruszwicka 10 - 28 parzyste, 33 - 53 nieparzyste, Litomska 10, 11, 20 - 36 parzyste, Poznańska 1 - 13 nieparzyste, Stefana Czarnieckiego 11 - 11D, 30 - 50 parzyste, Zachodnia 12 - 20 parzyste</t>
+  </si>
+  <si>
+    <t>Wrocław-Stare Miasto ulice: Drzewna, gen. Władysława Sikorskiego, Inowrocławska 23 - 39 nieparzyste, Jacka Kaczmarskiego, Rybacka, pl. Solidarności, pl. św. Mikołaja, Zachodnia 2, 4</t>
+  </si>
+  <si>
+    <t>Wrocław-Stare Miasto ulice: Inowrocławska 1 - 21D nieparzyste, 2 - 4 parzyste, Legnicka 17 - 27A nieparzyste, Młodych Techników 2 - 14 parzyste, 7, Szczepińska, Środkowa</t>
+  </si>
+  <si>
+    <t>Wrocław-Stare Miasto ulice: Braniborska 19 - 75 nieparzyste, 32 - 84 parzyste, Dobra 11 - 21 nieparzyste, Góralska, Legnicka 26 - 42 parzyste, Robotnicza 1 - 112, Smolecka, Trzemeska</t>
+  </si>
+  <si>
+    <t>Wrocław-Stare Miasto ulice: Aleksandra Zelwerowicza, Braniborska 1 - 7 nieparzyste, 2 - 30 parzyste, Dobra 2 - 16 parzyste, pl. Jana Pawła II 1, 2, Legnicka 16 - 24 parzyste, Marchijska, Nabycińska, pl. Orląt Lwowskich 1 - 20B, 20F, Podwale 1 - 25, Sokolnicza, Ziemowita, Wrocław-Fabryczna ulica Fabryczna 2 - 6 parzyste</t>
+  </si>
+  <si>
+    <t>Zespół Szkół nr 20, ul. Kłodnicka 36, 54-218 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Fabryczna ulice: Brynicka, Gądowska, Kłodnicka, Legnicka 118 - 168 parzyste, Małopanewska, Stobrawska, pl. Wiślany</t>
+  </si>
+  <si>
+    <t>Wrocław-Fabryczna ulice: Biały Kąt, Dąbrówki, Kwiska, Legnicka 50 - 116 parzyste</t>
+  </si>
+  <si>
+    <t>Wrocław-Fabryczna ulice: Bystrzycka 22 - 83, Na Ostatnim Groszu</t>
+  </si>
+  <si>
+    <t>Szkoła Podstawowa nr 118, bulw. Ikara 19, 54-130 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Fabryczna ulice: Eugeniusza Horbaczewskiego 3 - 43, płk. Bolesława Orlińskiego, Stefana Drzewieckiego 4 - 36D parzyste, Szybowcowa 1 - 14</t>
+  </si>
+  <si>
+    <t>Wrocław-Fabryczna ulica Jerzego Bajana 25 - 73</t>
+  </si>
+  <si>
+    <t>Wrocław-Fabryczna ulice: Czesława Tańskiego, Ludwika Idzikowskiego, Metalowców 61, Samolotowa, Skrzydlata, Sterowcowa</t>
+  </si>
+  <si>
+    <t>Wrocław-Fabryczna ulice: bulw. Dedala, Jerzego Bajana 1 - 24D, Stefana Drzewieckiego 3 - 35 nieparzyste</t>
+  </si>
+  <si>
+    <t>Wrocław-Fabryczna ulice: Latawcowa, Lotnicza 12 - 26 parzyste, 72, 100, 102, Szybowcowa 16 - 74 parzyste, 15 - 23 nieparzyste</t>
+  </si>
+  <si>
+    <t>Zespół Szkolno-Przedszkolny nr 2, ul. Eugeniusza Horbaczewskiego 61, 54-130 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Fabryczna ulice: Eugeniusza Horbaczewskiego 45 - 57A nieparzyste, bulw. Ikara, Stefana Drzewieckiego 65 - 71 nieparzyste</t>
+  </si>
+  <si>
+    <t>Wrocław-Fabryczna ulice: Balonowa, Bystrzycka 89 - 105, Eugeniusza Horbaczewskiego 59 - 75 nieparzyste</t>
+  </si>
+  <si>
+    <t>Wrocław-Fabryczna ulice: Franciszka Hynka, Stefana Drzewieckiego 38 - 64 parzyste, 41 - 63 nieparzyste</t>
+  </si>
+  <si>
+    <t>Zespół Szkolno-Przedszkolny nr 7, ul. Koszykarska 2 - 4, 54-134 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Fabryczna ulice: Aleja Śląska, Koszykarska, Mączna, Murarska, Notecka 3 - 7A nieparzyste, 4 - 16A parzyste, Papiernicza, Rękodzielnicza, Warciańska</t>
+  </si>
+  <si>
+    <t>Liceum Ogólnokształcące nr VI, ul. Hutnicza 45, 54-139 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Fabryczna ulice: Hutnicza, Nadrzeczna, Pilczycka 77 - 148B, Tkacka</t>
+  </si>
+  <si>
+    <t>Wrocław-Fabryczna ulice: Bednarska, Górnicza, Lotnicza 139 - 151 nieparzyste, 148 - 152 parzyste, Metalowców 9 - 11 nieparzyste, 25 - 31 nieparzyste, 59, 59B, 59C, Stargardzka, Szklarska</t>
+  </si>
+  <si>
+    <t>Wrocławski Klub "Anima", ul. Pilczycka 47, 54-150 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Fabryczna ulice: Kolista, Kozanowska 2, Lotnicza 7 - 11 nieparzyste, 37, 53, Modra 2 - 35, Pilczycka 25 - 65</t>
+  </si>
+  <si>
+    <t>Zespół Szkół nr 21, ul. Piotra Ignuta 28, 54-151 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Fabryczna ulice: Dokerska 3 - 37 nieparzyste, Gwarecka</t>
+  </si>
+  <si>
+    <t>Wrocław-Fabryczna ulice: Dokerska 2 - 54 parzyste, Piotra Ignuta, Sielska</t>
+  </si>
+  <si>
+    <t>Wrocław-Fabryczna ulice: Kozanowska 63 - 117, Modra 36 - 52</t>
+  </si>
+  <si>
+    <t>Szkoła Podstawowa nr 33, ul. Kolista 17, 54-152 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Fabryczna ulice: Dzielna 1 - 37, Gołężycka</t>
+  </si>
+  <si>
+    <t>Wrocław-Fabryczna ulice: Kozanowska 13 - 62, Pałucka, Wiślańska</t>
+  </si>
+  <si>
+    <t>Wrocław-Fabryczna ulice: Bobrzańska, Celtycka, Dobrzańska, Dziadoszańska, Dzielna 39 - 53, gen. Iwana Połbina, Setna, Ślężańska, Trzebowiańska</t>
+  </si>
+  <si>
+    <t>Szkoła Podstawowa nr 3, ul. Bobrza 27, 54-220 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Fabryczna ulice: Białowieska 2 - 54 parzyste, Bobrza 2 - 27, Rysia</t>
+  </si>
+  <si>
+    <t>Wrocław-Fabryczna ulice: Bobrza 28 - 44, Grobla Kozanowska, ks. Marcina Lutra, Milenijna 2, Wejherowska 3 - 77 nieparzyste, 34</t>
+  </si>
+  <si>
+    <t>Szkoła Podstawowa nr 5, ul. Jelenia 7, 54-242 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Fabryczna ulice: Legnicka 49 - 67 nieparzyste, Niedźwiedzia, Starograniczna, Żubrza</t>
+  </si>
+  <si>
+    <t>Wrocław-Fabryczna ulice: Białowieska 1 - 131 nieparzyste, 66 - 120 parzyste, Popowicka 1 - 63 nieparzyste, 2 - 60 parzyste</t>
+  </si>
+  <si>
+    <t>Wrocław-Fabryczna ulica Jelenia</t>
+  </si>
+  <si>
+    <t>Wrocław-Fabryczna ulice: Ojców Oblatów, Popowicka 62 - 158 parzyste, Wejherowska 2 - 28 parzyste, Zajęcza</t>
+  </si>
+  <si>
+    <t>Zespół Szkół nr 3, ul. Szkocka 64, 54-402 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Fabryczna ulica Strzegomska 46 - 56B parzyste, 85 - 145 nieparzyste, 138 - 322 parzyste</t>
+  </si>
+  <si>
+    <t>Wrocław-Fabryczna ulice: Estońska 40 - 44 parzyste, Szkocka 40 - 99C</t>
+  </si>
+  <si>
+    <t>Szkoła Podstawowa nr 28, ul. Grecka 59, 54-406 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Fabryczna ulice: Angielska, Australijska, Baskijska, Belgijska, Białoruska, Estońska 1 - 36, Francuska, Grecka, Holenderska, Irlandzka, Kanadyjska</t>
+  </si>
+  <si>
+    <t>Wrocław-Fabryczna ulice: Austriacka, Babimojska, Duńska, Fabryczna 10 - 33, Hiszpańska, Jana Szczyrki, Klecińska 87 - 155 nieparzyste, 124 - 214 parzyste, Muchoborska, Norweska, Nowosolska, Otyńska, Przemkowska, Rudzka, Stanów Zjednoczonych, Szkocka 1 - 35, Szwajcarska, Szwedzka, Traktatowa, Turecka, Ukraińska, Wagonowa</t>
+  </si>
+  <si>
+    <t>Wrocławski Klub Formaty, ul. Samborska 3 - 5, 54-615 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Fabryczna ulice: Aleksandra Godlewskiego, Graniczna 1, 2 - 10B parzyste, Heleny Boguszewskiej, Jana Parandowskiego, Janusza Meissnera, Jerzego Cieślikowskiego, Kamila Giżyckiego, Kazimierza Witalisa Szarskiego, Marii Dąbrowskiej, Marii Rodziewiczówny, Melchiora Wańkowicza, Otwocka, Romualda Cabaja, Stanisława Dygata, Tadeusza Dołęgi-Mostowicza, Witolda Gombrowicza, Zenona Kosidowskiego</t>
+  </si>
+  <si>
+    <t>Zespół Szkolno-Przedszkolny nr 15, ul. Stanisławowska 38 - 44, 54-611 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Fabryczna ulice: Bliźniacza, Dzielnicowa, Końcowa, Leopolda Tyrmanda, Osiedlowa, Pusta, Rejonowa, Sokalska, Stryjska, Trawowa, Zofii Kossak-Szczuckiej</t>
+  </si>
+  <si>
+    <t>Wrocław-Fabryczna ulice: Husycka, Ibn Siny Awicenny 1 - 9 nieparzyste, 12 - 22 parzyste, 37, Karpacka, Krzemieniecka, Łaska, Nowohucka, Pińska, Postępowa, Przedświt, Samborska, Słonimska, Stanisława Kunickiego, Tarnopolska, Żytomierska</t>
+  </si>
+  <si>
+    <t>Wrocław-Fabryczna ulice: Baranowicka, Drohobycka, Jurija Gagarina, Marka Hłaski, Podolska, al. Prezydenta Gabriela Narutowicza z wyłączeniem nr 20, Rakietowa 1 - 35, 38 - 44 parzyste, 50, Zbarska, Żwirki i Wigury, Żwirki i Wigury Zachodnia</t>
+  </si>
+  <si>
+    <t>Zespół Szkół nr 6, ul. Nowodworska 70 - 82, 54-438 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Fabryczna ulica Budziszyńska 76 - 135</t>
+  </si>
+  <si>
+    <t>Wrocław-Fabryczna ulica Rogowska 1 - 52A</t>
+  </si>
+  <si>
+    <t>Wrocław-Fabryczna ulice: Chociebuska, Gubińska, Rogowska 54 - 104, Strzegomska 193 - 201 nieparzyste, Sukielicka 28, Żernicka 74 - 88 parzyste</t>
+  </si>
+  <si>
+    <t>Wrocław-Fabryczna ulica Nowodworska</t>
+  </si>
+  <si>
+    <t>Liceum Ogólnokształcące nr XV, ul. Wojrowicka 58, 54-436 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Fabryczna ulice: Budziszyńska 1 - 74, Wojrowicka</t>
+  </si>
+  <si>
+    <t>Zespół Szkolno-Przedszkolny nr 1, ul. Zemska 16c, 54-438 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Fabryczna ulica Zemska 9 - 44B</t>
+  </si>
+  <si>
+    <t>Wrocław-Fabryczna ulice: Komorowska, Krośnieńska, Zemska 1 - 7</t>
+  </si>
+  <si>
+    <t>Wrocław-Fabryczna ulice: Grodecka, Rogowska 106 - 176</t>
+  </si>
+  <si>
+    <t>Rada Osiedla Kuźniki, ul. Sarbinowska 19 - 21, 54-320 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Fabryczna ulice: Bytowska, Darłowska, Domasławska, Dziwnowska, Elbląska, Gołnowska, Helska, Jaksonowicka, Knignicka, Koszalińska, Międzyzdrojska, Morska, Pucka, Pyrzycka, Sukielicka 1 - 13 nieparzyste, 4 - 16 parzyste, Uznamska, Wołyńska, Woźnicza, Żernicka 90 - 124 parzyste</t>
+  </si>
+  <si>
+    <t>Szkoła Podstawowa Nr 37, ul. Sarbinowska 10, 54-320 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Fabryczna ulice: Hermanowska, Sarbinowska</t>
+  </si>
+  <si>
+    <t>Wrocław-Fabryczna ulice: Dźwirzyńska, Kołobrzeska, Rewalska, Słupska, Świnoujska, Włodzimierza Majakowskiego</t>
+  </si>
+  <si>
+    <t>Rada Osiedla Żerniki, ul. Żernicka 219, 54-510 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Fabryczna ulice: Dojazd, Jerzmanowska 2 - 22 parzyste, 7 - 27 nieparzyste, Kiemliczów, Lubczykowa, Macieja Przybyły, Objazdowa, Osiniecka 1 - 22, Pieprzna, Przednia, Rumiankowa, Seweryna Udzieli, Strachowicka 1 - 45 nieparzyste, 2 - 50B parzyste, Żernicka 152 - 296 parzyste, 177 - 287 nieparzyste, Żurawinowa</t>
+  </si>
+  <si>
+    <t>Zespół Szkolno-Przedszkolny nr 10, ul. Rumiankowa 34, 54-512 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Fabryczna ulice: Adama Gdacjusza, Andrzeja Kmicica, Basi Wołodyjowskiej, Berberysowa, Graniczna 19 - 21A nieparzyste, Jagienki, Jana Amosa Komeńskiego, Jana Skrzetuskiego, Kardamonowa, Ketlinga, ks. Augustyna Kordeckiego, Onufrego Zagłoby, Rezedowa, Walentego Roździeńskiego</t>
+  </si>
+  <si>
+    <t>Rada Osiedla Jerzmanowo-Jarnołtów-Strachowice-Osiniec, ul. Jerzmanowska 102, 54-530 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Fabryczna ulice: Anny Jasińskiej, Aroniowa, Augustyna Kośnego, Cichociemnych, Desantowa, Gałowska, gen. Witolda Urbanowicza, Graniczna 16 - 32 parzyste, 85 - 163 nieparzyste, 183, 190, 201, Gromadzka 52, 52A, Gruszowa, Heleny i Ludwika Adamczewskich, Jana Karola Chodkiewicza, Jana Klemensa Branickiego, Janiny Kłopockiej, Jarnołtowska, Jerzmanowska 31 - 135, Kębłowicka, Kolendrowa, Koronna, Krobielowicka, Krzeptowska, ks. Bolesława Domańskiego, ks. Józefa Matuszka, Mikołaja Sieniawskiego, Osiniecka 46 - 124, Pawła Kwoczka, Piołunowa, Płużna, ppłk. Stanisława Skarżyńskiego, al. Prezydenta Gabriela Narutowicza nr 20, Rakietowa 37, 39, Rdestowa, Rodła, Samotworska, Sośnicka, Stanisława Jana Jabłonowskiego, Stanisława Koniecpolskiego, Stanisława Żółkiewskiego, Strachowicka 60 - 64 parzyste, 75 - 83 nieparzyste, Widłakowa, Władysława i Jana Wardzyńskich, Władysława Zarembowicza, Zbigniewa Brzezińskiego, Zofii Chrzanowskiej, Żwirowa 69 - 73L nieparzyste, 74</t>
+  </si>
+  <si>
+    <t>Ośrodek Postaw Twórczych Zamek, pl. Świętojański 1, 54-076 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Fabryczna ulice: Alojzego Majchra, Babiogórska, Beskidzka, Dukielska, Ekonomiczna, Gromadzka 1 - 49, 53 - 73D nieparzyste, Jajczarska, Józefa Gielniaka, al. Klonowa, Kosmonautów 206 - 328, Krajobrazowa, Logiczna, Malczycka, Matematyczna, Miodowa, Mleczarska, Panoramiczna, Pejzażowa, al. Platanowa, Plenerowa, Pustecka, Ratyńska, Równa, Serowarska, Snycerska, Stefana Batorego, Szkolna, pl. Świętojański, Trzmielowicka, Wojska Polskiego, Wyboista</t>
+  </si>
+  <si>
+    <t>Szkoła Podstawowa nr 95, ul. Starogajowa 66 - 68, 54-047 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Fabryczna ulice: Amarantowa, Biała, Bieszczadzka, Błękitna, Boguszowska, Ciechocińska, Cieplicka, Fioletowa, Granatowa, Iwonicka, Jeleniogórska, Jesiennicka, Kruszcowa, Lazurowa, Niecała, Pienińska, Skałeczna, Sobieszowska, Srebrzysta, Szara, Śnieżna, Tatrzańska, Zielona, Złota, Źródlana, Żółta</t>
+  </si>
+  <si>
+    <t>Szkoła Podstawowa nr 51, ul. Krępicka 50, 54-018 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Fabryczna ulice: Brzezińska, Bujna, Krępicka, Lubiąska, Małoszyńska, Młodzieżowa, Niemkińska, Niepierzyńska, Owczarska, Polkowicka, Prochowicka, Sosnowa, Szczepanowska, Woronowicka</t>
+  </si>
+  <si>
+    <t>Wrocław-Fabryczna ulice: Alfreda Jahna, Błońska, Borowikowa, Grzybowa, Hanny Wałkówskiej, Henryka Wereszyckiego, Iwo Jaworskiego, Jerzego Łanowskiego, Józefa Wąsowicza, Mariana Haisiga, Marszowicka 141 - 166, Marty Burbianki, Mieczysława Wolfkego, Modrzewiowa, Mokrzańska, Pawła Eluarda, Prężycka, Stanisława Bąka, Stanisława Hartmana, Teofila Modelskiego, Uraska, Władysława Czaplińskiego, Władysława Ślebodzińskiego, Zajazdowa</t>
+  </si>
+  <si>
+    <t>Wrocław-Fabryczna ulice: Jana Rubczaka, Kącka, Komornicka, Lubska, Lutyńska, Łączna, Michała Płońskiego, al. Prezydenta Ryszarda Kaczorowskiego 101, Promenada, Rytownicza, Stroma, Ślepa, Średzka, Władysława Skoczylasa, Wolska, Żarska</t>
+  </si>
+  <si>
+    <t>Zespół Szkolno-Przedszkolny nr 14, ul. Częstochowska 42, 54-031 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Fabryczna ulice: Bronowicka, Chęcińska, pl. Ciesielski, Grybowska, pl. Kaliski, Kielecka, Kościańska, Limanowska, Opoczyńska, Rawicka, Solińska, Tarnowska, Wielkopolska, Wschowska, Złotnicka, Żwirowa 1A - 35 nieparzyste, 2 - 36 parzyste, 58</t>
+  </si>
+  <si>
+    <t>Wrocław-Fabryczna ulice: Bocheńska, Częstochowska, Czorsztyńska, Dębicka, Halicka, Jarosławska, Jasielska, Nowosądecka, Nowotarska, Podhalańska, Przemyska, Rabczańska, Rzeszowska, Zakopiańska, Żywiecka</t>
+  </si>
+  <si>
+    <t>Wrocław-Fabryczna ulice: Beżowa, Cytrynowa, Drogosławicka, Figowa, gen. Augusta Emila Fieldorfa, Głuszycka, Jagniątkowska, Jeżowska, Mandarynkowa, Miłkowska, Mysłakowicka, Niebieska, Perłowa, Piechowicka, Pomarańczowa, Porębska, Przechodnia, Przesiecka, Purpurowa, Rodzynkowa, Seledynowa, Stabłowicka 1 - 74, 76 - 88 parzyste, Starogajowa, Staroleska, Szkarłatna</t>
+  </si>
+  <si>
+    <t>Wrocław-Fabryczna ulice: Arachidowa, Będkowska, Jaźwińska, Jędrzejowska, Olbrachtowska, Piotrkowska, Stoszowska, Strzeblowska, Sulistrowska, Wojanowska</t>
+  </si>
+  <si>
+    <t>Wrocław-Fabryczna ulice: Ananasowa, Białkowska, Bojanowska, Chocianowska, Chwalimierska, Chwałkowska 9 - 16, Dłużycka, Dziarska, Głębowicka, Główna 146 - 151, Górecka 2, 1 - 165 nieparzyste, 38 - 118 parzyste, Grębocicka, Gwizdanowska, Hodowicka, Jana Mydlarskiego, Krzelowska, Krzyżowska, Lubawska, Łososiowicka, Malownicza, Małomicka, Marii i Stanisława Dawskich, Marszowicka 1 - 131, Mrozowska, Ochocza, Pisarzowicka, Przemiłowska, Rychła, Sieroszowicka, Starobielawska 53A, 59A, Świeża, Uciechowska, Wełniana 3 - 67 nieparzyste, 4 - 68 parzyste, Wilkszyńska, Wojnowicka, Wróblowicka, Zebrzydowska</t>
+  </si>
+  <si>
+    <t>Dolnośląski Specjalny Ośrodek Szkolno-Wychowawczy nr 13 dla Uczniów Niewidomych i Słabowidzących oraz z innymi niepełnosprawnościami im. Marii Grzegorzewskiej we Wrocławiu, ul. Kamiennogórska 16, 54-034 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Fabryczna ulice: Andrzeja Frydeckiego, al. Architektów, Białodrzewna, Białogardzka, Bukowa, Ernsta Maya, Grabowa, Hansa Poelziga, Heinricha Lauterbacha, Igora Tawryczewskiego, Kazimierza Bieńkowskiego, Konińska, Krystyny i Mariana Barskich, Lewa, Maxa Berga, Mieczysława Zlata, pasaż Adolfa Radinga, Ryżowa, Szczecińska 5 - 21B nieparzyste, Tadeusza Brzozy, Trójkątna, Witolda Lipińskiego, Żernicka 299</t>
+  </si>
+  <si>
+    <t>Zespół Szkolno-Przedszkolny nr 12, ul. Lubelska 95a, 54-101 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Fabryczna ulice: Białostocka, Biłgorajska, Brodzka 5 - 81 nieparzyste, Chełmska, Ciechanowska, Lubelska, Łukowska, Nałęczowska, Potokowa, Północna, Radzyńska, Ruczajowa, Siedlecka, Stodolna, Tykocińska, Zamojska</t>
+  </si>
+  <si>
+    <t>Zespół Szkolno-Przedszkolny nr 12, ul. Suwalska 5, 54-104 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Fabryczna ulice: Braniewska, Brodnicka, Gminna, Hodowlana, Iławska, Królewiecka, Narzędziowa, Sadownicza, Suwalska</t>
+  </si>
+  <si>
+    <t>Wrocław-Fabryczna ulice: Augustowska, Dworska, Fromborska, Gosławicka, Lidzbarska, Ługowińska, Mrągowska, Nasienna, Notecka 9 - 15 nieparzyste, 18, Paniowicka, Pilczycka 156 - 205, Rędzińska, Rolna, Warmińska, Węgliniecka</t>
+  </si>
+  <si>
+    <t>Wrocław-Fabryczna ulice: Maślicka 1 - 104, Michała Wołodyjowskiego, Ostródzka, Pasieczna, Pasłęcka, Pasymska, Reszelska, Ślęzoujście, al. Śliwowa, Tolkmicka, Wilkaska, Żytawska</t>
+  </si>
+  <si>
+    <t>Zespół Szkolno-Przedszkolny nr 20, ul. Karpnicka 2, 54-061 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Fabryczna ulice: Chwałkowska 1 - 7, Górecka 4 - 16 parzyste, Jodłowicka, Lubomierska, Polonii Wrocławskiej, Pracka, Starobielawska 1 - 53 nieparzyste, 2 - 52 parzyste, 53C - 59 nieparzyste, 61 - 69 nieparzyste, Towarowa, Wełniana 69 - 75, Włókniarzy, Zbożowa</t>
+  </si>
+  <si>
+    <t>Wrocław-Fabryczna ulice: Brodzka 10 - 10F parzyste, 131 - 203 nieparzyste, 142 - 208 parzyste, Cukiernicza, Edmunda Osmańczyka, Franciszka Juszczaka, Gryczana, Imbirowa, Jaglana, Janowska, Karczemna, Karpnicka, Kukurydziana, Łomnicka, Orkiszowa, Otrębowa, Piekarska, Piwowarska, Urodzajna</t>
+  </si>
+  <si>
+    <t>Liceum Ogólnokształcące nr XIV, al. Aleksandra Brücknera 10, 51-410 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Psie Pole ulice: al. Aleksandra Brücknera 10 - 54 parzyste, Bolesława Krzywoustego 1 - 109, 111, Giżycka, Grudziądzka, Kętrzyńska, al. Poprzeczna 33/35, 33A, Toruńska</t>
+  </si>
+  <si>
+    <t>Szkoła Podstawowa nr 83, al. Tadeusza Boya-Żeleńskiego 32, 51-160 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Psie Pole ulice: Adolfa Dygasińskiego, Bydgoska, Galla Anonima, Jana Długosza, Kazimierza Przerwy-Tetmajera, Łąka Mazurska, Macieja Miechowity, al. Marcina Kromera, al. Tadeusza Boya-Żeleńskiego, Tadeusza Micińskiego, Wacława Berenta, Wacława Potockiego, Władysława Orkana</t>
+  </si>
+  <si>
+    <t>Szkoła Podstawowa nr 83, ul. Stanisława Przybyszewskiego 59, 51-151 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Psie Pole ulice: Adama Asnyka, Bolesława Leśmiana, bp. Ignacego Krasickiego, Franciszka Karpińskiego, gen. Józefa Wybickiego, pl. Gustawa Daniłowskiego, al. Jana Kasprowicza 34 - 112, Juliana Klaczki, Leopolda Staffa, Ludwika Nabielaka, pl. marsz. Józefa Piłsudskiego, Stanisława Piętaka, Stanisława Przybyszewskiego, Tadeusza Zelenaya, Teofila Lenartowicza, Zenona Miriama Przesmyckiego</t>
+  </si>
+  <si>
+    <t>Szkoła Podstawowa Nr 83, al. Tadeusza Boya-Żeleńskiego 32, 51-160 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Psie Pole ulice: Artura Oppmana, Bohdana Zaleskiego, Filomatów, Ignacego Chrzanowskiego, Jana Brzechwy, Kornela Makuszyńskiego, Kornela Ujejskiego, ks. Norberta Bonczyka, Marii Konopnickiej, Samuela Bogumiła Lindego, Seweryna Goszczyńskiego, Skwer Obrońców Helu, Stanisława Grochowiaka, Tadeusza Gajcego, Wacława Gąsiorowskiego, Wincentego Pola 1 - 63 nieparzyste, 2 - 48C parzyste, Władysława Anczyca, Władysława Syrokomli, Włodzimierza Perzyńskiego</t>
+  </si>
+  <si>
+    <t>Szkoła Podstawowa Nr 83, ul. Stanisława Przybyszewskiego 59, 51-151 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Psie Pole ulica Piotra Czajkowskiego</t>
+  </si>
+  <si>
+    <t>Wrocław-Psie Pole ulice: Artyleryjska, Koszarowa, Sołtysowicka 1 - 5A nieparzyste, 2 - 12 parzyste, 15 - 24, Sportowa</t>
+  </si>
+  <si>
+    <t>Szkoła Podstawowa nr 20, ul. Henryka Michała Kamieńskiego 24, 51-124 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Psie Pole ulice: Forteczna, Jutrosińska, Kazimierza Brodzińskiego, Krzysztofa Kamila Baczyńskiego, Maurycego Mochnackiego, Mieczysława Romanowskiego, Roberta Kocha, Torowa, Wincentego Pola 50 - 70 parzyste, 65 - 77A nieparzyste, Żmigrodzka 9 - 36</t>
+  </si>
+  <si>
+    <t>Wrocław-Psie Pole ulice: Henryka Michała Kamieńskiego 3 - 184, Kępińska, Ligocka, Paprotna 2 - 6, Wołowska, Żmigrodzka 38 - 145</t>
+  </si>
+  <si>
+    <t>Szkoła Podstawowa Nr 50, ul. Czeska 38, 51-112 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Psie Pole ulice: al. Jana Kasprowicza 1 - 33, Rowerowa, Władysława Broniewskiego, Zawalna</t>
+  </si>
+  <si>
+    <t>Wrocław-Psie Pole ulice: Młynarska, Teodora Parnickiego, Zaułek Rogoziński</t>
+  </si>
+  <si>
+    <t>Szkoła Podstawowa nr 50, ul. Czeska 38, 51-112 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Psie Pole ulice: Bałkańska, Bałtycka, Bułgarska, Czeska, Jarocińska 99, Lutycka, Łużycka, Morawska, Obodrzycka, Osobowicka 2 - 63, Serbska, Słowacka, Weroniki Kumko</t>
+  </si>
+  <si>
+    <t>Liceum Ogólnokształcące nr X, ul. Piesza 1, 51-109 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Psie Pole ulica Obornicka 2 - 76F</t>
+  </si>
+  <si>
+    <t>Wrocław-Psie Pole ulice: Macedońska, Na Polance, Piesza</t>
+  </si>
+  <si>
+    <t>Szkoła Podstawowa Nr 50, ul. Czeska 40, 51-112 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Psie Pole ulica Jugosłowiańska</t>
+  </si>
+  <si>
+    <t>Wrocław-Psie Pole ulica Bezpieczna</t>
+  </si>
+  <si>
+    <t>Wrocław-Psie Pole ulica Chorwacka</t>
+  </si>
+  <si>
+    <t>Szkoła Podstawowa nr 8, ul. Kowalska 105, 51-424 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Psie Pole ulice: Bociania, Chłopska, Czajcza, Działdowska, Ełcka, Gołdapska, Grajewska, Kowalska, Lechitów, Łabędzia, Mokra, Monopolowa, Mydlana 2 - 2B, Niborska, Olsztyńska, Rakowa, Szczycieńska, Tczewska, Wenedów, Węgoborska, Wilgotna, Włodarska</t>
+  </si>
+  <si>
+    <t>Wrocław-Psie Pole ulice: al. Aleksandra Brücknera 23 - 55 nieparzyste, Bażancia, Bolesława Krzywoustego 110/118, 115 - 184, Gęsia, Gołębia, al. Jana Kochanowskiego 91B, 93, Jaskółcza, Kościerzyńska, Kukułcza, Kuropatwia, Kwidzyńska, Mewia, al. Poprzeczna 72 - 86 parzyste, Sikorcza, Szczygla, Szpacza, Wilgowa, Wronia</t>
+  </si>
+  <si>
+    <t>Szkoła Podstawowa nr 6, ul. Gorlicka 25, 51-314 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Psie Pole ulice: Bławatna, Dłutowa, Grodzieńska, Iwana Franki, Jana Palacha, Kordiana, Kowieńska, Kurlandzka, Lidzka, Malborska, Mazepy, Miejska, Mroźna, Nadbrzeżna, Nowogródzka, Rzeczna, Sienna, Tarasa Szewczenki, Trocka, Witebska</t>
+  </si>
+  <si>
+    <t>Zespół Szkolno-Przedszkolny nr 3, ul. Inflancka 13, 51-354 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Psie Pole ulica Litewska</t>
+  </si>
+  <si>
+    <t>Wrocław-Psie Pole ulice: Poleska 1 - 32A, Żmudzka</t>
+  </si>
+  <si>
+    <t>Wrocław-Psie Pole ulice: Inflancka, Poleska 33 - 50</t>
+  </si>
+  <si>
+    <t>Wrocław-Psie Pole ulice: Czernicka, Kiełczowska 31 - 177, Miłostowska, Mirkowska</t>
+  </si>
+  <si>
+    <t>Szkoła Podstawowa nr 98, ul. Sycowska 22a, 51-319 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Psie Pole ulice: Białych Goździków, Bolesława Krzywoustego 250 - 334, Czerwonej Róży, Czerwonych Maków, Dobroszycka, al. Jana III Sobieskiego, Kłokoczycka, mjr. Jana Piwnika-Ponurego, Polnych Niezapominajek, Zakrzowska, Złotej Lilii</t>
+  </si>
+  <si>
+    <t>Wrocław-Psie Pole ulice: Bierutowska, Sycowska, Zielna</t>
+  </si>
+  <si>
+    <t>Wrocław-Psie Pole ulice: Bylinowa, Farna, Gorlicka, Kiełczowska 1, 15, 10 - 30C parzyste, ks. Mariana Stanety, Mulicka, Rycerska, Tylna, Wójtowska</t>
+  </si>
+  <si>
+    <t>Szkoła Podstawowa nr 44, ul. Wilanowska 31, 51-206 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Psie Pole ulice: Chocimska, Hetmańska, Kasztelańska, Oleska, Wiedeńska, Zatorska 110 - 144 parzyste, Zofii Gumińskiej</t>
+  </si>
+  <si>
+    <t>Wrocław-Psie Pole ulice: Belgradzka, Brzuchowicka, Charkowska, Danuty Siedzikówny, Heleny Motykówny, Królewska, Królowej Marysieńki, Kurska, Liońska, Łuczników, Odeska, Omska, Paryska, Ryska, Sewastopolska, Staropolska, Tallińska, Wilanowska, Wołgogradzka</t>
+  </si>
+  <si>
+    <t>Fundacja PRZYJAZNY DOM im. Stanisława Jabłonki, ul. gen. Leopolda Okulickiego 2, 51-216 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Psie Pole ulice: Archeologów, Etnografów, gen. Leopolda Okulickiego, Gostyńska, Jagiellońska, Kotwiczna, Księżycowa, Łozińska, Marynarska, Niepodległości, Odolanowska, Odrodzenia Polski, Orna, Skarbu Zakrzowskiego, Spacerowa, Stoczniowa</t>
+  </si>
+  <si>
+    <t>Publiczna Szkoła i Przedszkole MARCO POLO, ul. Zatorska 11, 51-215 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Psie Pole ulice: Bratysławska, Chmielna, Dubrownicka, gen. Stanisława Kopańskiego, gen. Tadeusza Bora-Komorowskiego, Irkucka, Konrada Wallenroda, Lublańska, Masztowa, Okrętowa, Pedagogiczna, Przedwiośnie 1 - 5A nieparzyste, 2B, Sarajewska, Skopijska, Wilczkowska, Zagrzebska, Zatorska 1 - 108H</t>
+  </si>
+  <si>
+    <t>Zespół Szkolno-Przedszkolny nr 23, ul. Przedwiośnie 47, 51-211 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Psie Pole ulice: Astrowa, Azaliowa, Barwinkowa, Bratkowa, Daliowa, Forsycjowa, Frezjowa, Groszkowa 1 - 16, Hiacyntowa, Jaśminowa, Jeziorowa, Konwaliowa, Krokusowa, Kwiatowa, Liliowa, Maciejkowa, Macierzankowa, Malwowa, Mieczykowa, Mirtowa, Nagietkowa, Pawłowicka, Przebiśniegowa, Przedwiośnie 2, 2A, 2AB, 5F - 88, Przylaszczkowa, Ruciana, Sasankowa, Starodębowa, Stokrotkowa, Szafranowa, Szarotkowa, Widawska, Zawilcowa 10, Złocieniowa, Żonkilowa</t>
+  </si>
+  <si>
+    <t>Zespół Szkolno-Przedszkolny nr 4 (Szkoła Podstawowa nr 40), ul. Sołtysowicka 34, 51-168 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Psie Pole ulice: Bagatela, Bombardierska, Bronisława Knastera, Lekcyjna, Edwarda Marczewskiego, Elementarzowa, Gimnazjalna, al. Poprzeczna 1, 37 - 68A, Przejazdowa, Redycka 1 - 90, Strzelecka</t>
+  </si>
+  <si>
+    <t>Wrocław-Psie Pole ulice: Czytankowa, Fortowa, Kanonierska, Lothara Herbsta, Mariana Falskiego, płk. Ryszarda Kuklińskiego, Rafała Wojaczka, Sołtysowicka 11 - 11C nieparzyste, 13/15, 25 - 73, Torfowa</t>
+  </si>
+  <si>
+    <t>Pensjonat dla Osób Starszych i z Niepełnosprawnościami, ul. Henryka Michała Kamieńskiego 190, 51-124 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Psie Pole ulice: Bukowicka, Henryka Michała Kamieńskiego 188 - 278BB, Korzeńska, Milicka, Osiecka, Pakosławska, Paprotna 7 - 16A, Postolińska, Prusicka, Rudawska, Sakury, Sulejowska, Sulmierzycka, Twardogórska, Wierzchowicka, Złotowska</t>
+  </si>
+  <si>
+    <t>Świetlica Osiedlowa Rady Osiedla Polanowice-Poświętne-Ligota, ul. Henryka Michała Kamieńskiego 256, 51-180 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Psie Pole ulice: Ałunowa, Aptekarska, Białych Tygrysów, Bierzycka, Brzostowska, Cerekwicka, Domanowicka, Hugona Kowarzyka, Irysowa, Kazimierza Funka, Kątowa, Krośnicka, Krzyżanowicka, Lekarska, Ludwika Kubali, Ługowa, Machnicka, Michała Tadeusza Falzmanna 1 - 16, Osolska, Polanowicka, Poświęcka, Ramiszowska, Raszowska, Redycka 128 - 141, Skoczna, Skoroszowska, Starościńska, Stradomska, Zawońska, Żmigrodzka 183 - 257A</t>
+  </si>
+  <si>
+    <t>Siedziba Rady Osiedla Widawa, ul. Kominiarska 68, 51-180 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Psie Pole ulice: Aleksandra Szniolisa, Cholewkarska, Dekarska, Fryzjerska, Geodezyjna, Grawerska, Haliny Konopackiej, Jubilerska, Kaletnicza, Kminkowa 66 - 89, Kominiarska 15 - 98, Księgarska, Lawendowa 6 - 10 parzyste, Łopianowa, Meliorancka, Meliorancka Południowa, Melisowa 14 - 30 parzyste, 50, Miętowa 4 - 8 parzyste, Ostowa Północna, Pielęgniarska, Polanowicka Północna, Rzemieślnicza, Strażacka, Sułowska, Szkutnicza, Zduńska, Zecerska, Zegarmistrzowska, Zygmunta Markowskiego</t>
+  </si>
+  <si>
+    <t>Rada Osiedla Lipa Piotrowska, ul. Tymiankowa 3, 51-180 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Psie Pole ulice: Bazyliowa, Cynamonowa, Ćwiczebna 1 - 11 nieparzyste, Heleny Marusarzówny, Jałowcowa, Kaczeńcowa, Kaparowa, Kominiarska 1 - 14, Korzenna, Kurkumowa 3, Laurowa, Lawendowa 3 - 23 nieparzyste, 22 - 24 parzyste, Lukrecjowa, Majerankowa, Melisowa 1 - 33 nieparzyste, Miętowa 1 - 9 nieparzyste, Miętowa Południowa, Obornicka 235A, 237, Ostowa, Podbiałowa, Szałwiowa, Waniliowa</t>
+  </si>
+  <si>
+    <t>Rada Osiedla Świniary, ul. Pęgowska 14, 51-180 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Psie Pole ulice: Anyżowa, Bakaliowa, Czarnuszkowa, Dalimira, Gorczycowa, Kminkowa 6, 10, 18 - 64, Koperkowa, Mikory, Pełczyńska, Perzowa, Pęgowska, Pokrzywowa, Szczawiowa, Tymiankowa, Zabłocie, Zagaje, Zajączkowska, Zalipie, Załęże, Zamłynie, Zapotocze, Zarzecze, Zaziębie</t>
+  </si>
+  <si>
+    <t>Zespół Szkolno-Przedszkolny nr 5, ul. Osobowicka 127, 51-004 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Psie Pole ulice: Ćwiczebna 100 - 105, Edmonda Micheleta, Edytorska, Hokeistów, Inspektowa, Jana Kuglina, Jarocińska 6 - 74, Kajakarzy, Kapliczna, Koszykarzy, Krotoszyńska, Lipska, Łyżwiarzy, Opłotkowa, Osobowicka 70 - 177, Ostrowska, Ostrzeszowska, Palisadowa, Piłkarzy, Rodziny Kornów, Siatkarzy, Szachistów, Szczypiornicka, Ślazowa, Śremska, św. Huberta, Wędkarzy, Wieluńska, Wieruszowska, Witkowska, Wrzosowa, pl. Wyzwolenia, Żużlowców, Żywopłotowa</t>
+  </si>
+  <si>
+    <t>Centrum GRAFIT, ul. Namysłowska 8, 50-304 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Psie Pole ulice: Antoniego Słonimskiego, Browarna, Rychtalska 7 - 24, Zakładowa</t>
+  </si>
+  <si>
+    <t>Wrocław-Krzyki ulice: Adama Uznańskiego, Jerzego Kukuczki, Kłodzka, Srebrnogórska</t>
+  </si>
+  <si>
+    <t>Wrocław-Krzyki ulica: Piękna</t>
+  </si>
+  <si>
+    <t>Wrocław-Krzyki ulice: Opolska 1 - 99, Turawska, Tyska, Bytomska, Gogolińska, Leona Popielskiego, Myszkowska, Siewierska, Sosnowiecka</t>
+  </si>
+  <si>
+    <t>Zespół Szkolno-Przedszkolny nr 25, ul. Asfaltowa 6, 52-235 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Krzyki ulice: Adama Kopycińskiego, Ady Sari, Barbary Kostrzewskiej, Beaty Artemskiej, Grażyny Bacewicz, Rafała Maszkowskiego, Stanisława Drabika, Wojciecha Kilara</t>
+  </si>
+  <si>
+    <t>Wrocław-Krzyki ulice: Barbary Hesse-Bukowskiej, Krzysztofa Komedy, Edmunda Kajdasza, Franciszki Platówny, Haliny Halskiej, Henryka Jareckiego 3 - 11 nieparzyste, 6 - 24C parzyste, Jana Kiepury, Jerzego Gardy, Sarnia, Wspólna 49 - 81 nieparzyste</t>
+  </si>
+  <si>
+    <t>Wrocław-Krzyki ulice: Jeździecka, Partynicka, Zwycięska</t>
+  </si>
+  <si>
+    <t>Zespół Szkolno-Przedszkolny nr 15, ul. Stanisławowska 38-44, 54-611 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Fabryczna ulice: Antoniego Knota, Buczacka, Mińska, Roślinna, Stanisławowska, Włodzimierza Trzebiatowskiego, Zagony</t>
+  </si>
+  <si>
+    <t>Wrocław-Fabryczna ulice: Chobieńska, Dolnobrzeska, Iglasta, Junacka, Kresowa, Liściasta, Mojęcicka, Ostrężynowa, Smolna, Szpilkowa, Świerkowa, Ulowa, Watowa, Wińska</t>
+  </si>
+  <si>
+    <t>Wrocław-Fabryczna ulice: Kamiennogórska, Krzeszowska, Łukowa, Małopolska, Miechowska, Mieroszowska, Olkuska, Radomska, Rajska</t>
+  </si>
+  <si>
+    <t>Wrocław-Fabryczna ulice: Arbuzowa, Daktylowa, Hoża, Kokosowa, Oliwkowa, Samotna</t>
+  </si>
+  <si>
+    <t>Wrocław-Fabryczna ulice: Bogatyńska, Kozia, Łomżyńska, Maślicka 138-219, Porajowska, Turoszowska, Zawidowska</t>
+  </si>
+  <si>
+    <t>Wrocław-Fabryczna ulice: Główna 1 - 93 nieparzyste, 6 - 102 parzyste, Stabłowicka 75 - 149 nieparzyste, 98 - 168 parzyste</t>
+  </si>
+  <si>
+    <t>Wrocław-Psie Pole ulica Obornicka 77A - 235</t>
+  </si>
+  <si>
+    <t>Siedziba Rady Osiedla Polanowice-Poświętne-Ligota, ul. Henryka Michała Kamieńskiego 190, 51-124 Wrocław</t>
+  </si>
+  <si>
+    <t>Wrocław-Psie Pole ulice: Adama Jerzego Czartoryskiego, Michała Tadeusza Falzmanna 17 - 33, Pleszewska</t>
+  </si>
+  <si>
+    <t>Zakład Opiekuńczo-Leczniczy o Profilu Rehabilitacyjnym Zgromadzenia Sióstr Św. Elżbiety, ul. św. Józefa 2/4, 50-329 Wrocław</t>
+  </si>
+  <si>
+    <t>Zakład Opiekuńczo-Leczniczy o Profilu Rehabilitacyjnym Zgromadzenia Sióstr Św. Elżbiety</t>
+  </si>
+  <si>
+    <t>Areszt Śledczy we Wrocławiu, ul. Świebodzka 1, 50-046 Wrocław</t>
+  </si>
+  <si>
+    <t>Areszt Śledczy we Wrocławiu</t>
+  </si>
+  <si>
+    <t>Dolnośląskie Centrum Onkologii, Pulmonologii i Hematologii we Wrocławiu, ul. Grabiszyńska 105, 53-439 Wrocław</t>
+  </si>
+  <si>
+    <t>Dolnośląskie Centrum Onkologii, Pulmonologii i Hematologii we Wrocławiu</t>
+  </si>
+  <si>
+    <t>Oddział Zewnętrzny Aresztu Śledczego we Wrocławiu, ul. Fiołkowa 38, 53-239 Wrocław</t>
+  </si>
+  <si>
+    <t>Oddział Zewnętrzny Aresztu Śledczego we Wrocławiu</t>
+  </si>
+  <si>
+    <t>Samodzielny Publiczny Zakład Opieki Zdrowotnej MSWiA we Wrocławiu, ul. Ołbińska 32, 50-233 Wrocław</t>
+  </si>
+  <si>
+    <t>Samodzielny Publiczny Zakład Opieki Zdrowotnej MSWiA we Wrocławiu</t>
+  </si>
+  <si>
+    <t>"Dolnośląskie Centrum Zdrowia Psychicznego" sp. z o. o., wyb. Józefa Conrada-Korzeniowskiego 18, 50-226 Wrocław</t>
+  </si>
+  <si>
+    <t>"Dolnośląskie Centrum Zdrowia Psychicznego" sp. z o. o.</t>
+  </si>
+  <si>
+    <t>Zakład Karny Nr 1 we Wrocławiu, ul. Kleczkowska 35, 50-211 Wrocław</t>
+  </si>
+  <si>
+    <t>Zakład Karny Nr 1 we Wrocławiu</t>
+  </si>
+  <si>
+    <t>Uniwersytecki Szpital Kliniczny im. Jana Mikulicza-Radeckiego we Wrocławiu, sala wykładowa Nyska, wyb. Ludwika Pasteura 4, 50-367 Wrocław</t>
+  </si>
+  <si>
+    <t>Uniwersytecki Szpital Kliniczny im. Jana Mikulicza-Radeckiego we Wrocławiu</t>
+  </si>
+  <si>
+    <t>Dolnośląskie Centrum Onkologii, Pulmonologii i Hematologii we Wrocławiu, pl. Ludwika Hirszfelda 12, 53-413 Wrocław</t>
+  </si>
+  <si>
+    <t>4. Wojskowy Szpital Kliniczny z Polikliniką SP ZOZ we Wrocławiu, ul. Rudolfa Weigla 5, 53-114 Wrocław</t>
+  </si>
+  <si>
+    <t>4. Wojskowy Szpital Kliniczny z Polikliniką SP ZOZ we Wrocławiu</t>
+  </si>
+  <si>
+    <t>Uniwersytecki Szpital Kliniczny im. Jana Mikulicza-Radeckiego we Wrocławiu-budynek H, sala wykładowa nr 3/48, ul. Borowska 213, 50-556 Wrocław</t>
+  </si>
+  <si>
+    <t>Uniwersytecki Szpital Kliniczny im. Jana Mikulicza-Radeckiego we Wrocławiu-budynek H</t>
+  </si>
+  <si>
+    <t>Uniwersytecki Szpital Kliniczny im. Jana Mikulicza-Radeckiego we Wrocławiu-budynek J, sala wykładowa nr 1/182, ul. Borowska 213, 50-556 Wrocław</t>
+  </si>
+  <si>
+    <t>Uniwersytecki Szpital Kliniczny im. Jana Mikulicza-Radeckiego we Wrocławiu-budynek J</t>
+  </si>
+  <si>
+    <t>ORPEA Polska Sp. z o.o. Rezydencja przy Dyrekcyjnej, ul. Dyrekcyjna 5-7, 50-528 Wrocław</t>
+  </si>
+  <si>
+    <t>ORPEA Polska Sp. z o.o. Rezydencja przy Dyrekcyjnej</t>
+  </si>
+  <si>
+    <t>Dom Pomocy Społecznej "Samarytanin", ul. Świątnicka 25/27, 52-018 Wrocław</t>
+  </si>
+  <si>
+    <t>Dom Pomocy Społecznej "Samarytanin"</t>
+  </si>
+  <si>
+    <t>Szpital Specjalistyczny im. A. Falkiewicza, ul. Warszawska 2, 52-114 Wrocław</t>
+  </si>
+  <si>
+    <t>Szpital Specjalistyczny im. A. Falkiewicza</t>
+  </si>
+  <si>
+    <t>Dom Pomocy Społecznej, ul. Karmelkowa 25, 52-437 Wrocław</t>
+  </si>
+  <si>
+    <t>Dom Pomocy Społecznej</t>
+  </si>
+  <si>
+    <t>Dom Pomocy Społecznej, ul. Mączna 3, 54-131 Wrocław</t>
+  </si>
+  <si>
+    <t>Dom Pomocy Społecznej "Miłosierny Samarytanin", ul. ks. Marcina Lutra 2-8, 54-239 Wrocław</t>
+  </si>
+  <si>
+    <t>Dom Pomocy Społecznej "Miłosierny Samarytanin"</t>
+  </si>
+  <si>
+    <t>Dolnośląski Szpital Specjalistyczny im. T. Marciniaka-Centrum Medycyny Ratunkowej, ul. gen. Augusta Emila Fieldorfa 2, 54-049 Wrocław</t>
+  </si>
+  <si>
+    <t>Dolnośląski Szpital Specjalistyczny im. T. Marciniaka-Centrum Medycyny Ratunkowej</t>
+  </si>
+  <si>
+    <t>Dom Pomocy Społecznej, ul. Rędzińska 66/68, 54-106 Wrocław</t>
+  </si>
+  <si>
+    <t>Wojewódzki Szpital Specjalistyczny im. J. Gromkowskiego, ul. Koszarowa 5, 51-149 Wrocław</t>
+  </si>
+  <si>
+    <t>Wojewódzki Szpital Specjalistyczny im. J. Gromkowskiego</t>
+  </si>
+  <si>
+    <t>Dom Pomocy Społecznej "Arka" i Dom Pomocy Społecznej "Arka 2", Zespół Mieszkań Wspomagających, ul. Jutrosińska 29, 51-124 Wrocław</t>
+  </si>
+  <si>
+    <t>Dom Pomocy Społecznej "Arka" i Dom Pomocy Społecznej "Arka 2"; Zespół Mieszkań Wspomagających</t>
+  </si>
+  <si>
+    <t>Wojewódzki Szpital Specjalistyczny we Wrocławiu, ul. Henryka Michała Kamieńskiego 73a, 51-124 Wrocław</t>
+  </si>
+  <si>
+    <t>Wojewódzki Szpital Specjalistyczny we Wrocławiu</t>
+  </si>
+  <si>
+    <t>Dolnośląskie Centrum Chorób Serca im. prof. Zbigniewa Religi-Medinet Sp. z o. o., ul. Henryka Michała Kamieńskiego 73a, 51-124 Wrocław</t>
+  </si>
+  <si>
+    <t>Dolnośląskie Centrum Chorób Serca im. prof. Zbigniewa Religi-Medinet Sp. z o. o.</t>
+  </si>
+  <si>
+    <t>Szpital Rehabilitacyjny Provita, ul. Bierutowska 63, 51-317 Wrocław</t>
+  </si>
+  <si>
+    <t>Szpital Rehabilitacyjny Provita</t>
+  </si>
+  <si>
+    <t>Wojewódzki Szpital Specjalistyczny we Wrocławiu-Zamiejscowy Oddział Rehabilitacyjny, ul. Poświęcka 8, 51-128 Wrocław</t>
+  </si>
+  <si>
+    <t>Wojewódzki Szpital Specjalistyczny we Wrocławiu-Zamiejscowy Oddział Rehabilitacyjny</t>
+  </si>
+  <si>
+    <t>Vratislavia Medica Szpital im. Św. Jana Pawła II, ul. Lekarska 1, 51-134 Wrocław</t>
+  </si>
+  <si>
+    <t>Vratislavia Medica Szpital im. Św. Jana Pawła II</t>
+  </si>
+  <si>
+    <t>Dom Pomocy Społecznej, ul. Kaletnicza 8, 51-180 Wrocław</t>
+  </si>
+  <si>
+    <t>ORPEA Polska Sp. z o. o. Rezydencja Św. Jadwiga, ul. gen. Kazimierza Pułaskiego 4, 50-446 Wrocław</t>
+  </si>
+  <si>
+    <t>ORPEA Polska Sp. z o. o. Rezydencja Św. Jadwiga</t>
   </si>
 </sst>
 </file>
@@ -873,9 +1956,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D102"/>
+  <dimension ref="A1:D331"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A326" workbookViewId="0">
+      <selection activeCell="C343" sqref="C343"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2299,12 +3384,3459 @@
         <v>100</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="2"/>
-      <c r="B102" s="2"/>
-      <c r="C102" s="2"/>
+    <row r="102" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A102" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="D102" s="3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A103" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="D103" s="3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A104" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="D104" s="3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A105" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="D105" s="3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A106" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="D106" s="3">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A107" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="D107" s="3">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A108" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D108" s="3">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A109" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="D109" s="3">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A110" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="D110" s="3">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A111" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="D111" s="3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A112" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="D112" s="3">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A113" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C113" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="D113" s="3">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A114" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D114" s="3">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A115" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D115" s="3">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A116" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C116" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="D116" s="3">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A117" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C117" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="D117" s="3">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A118" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="D118" s="3">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A119" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C119" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="D119" s="3">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A120" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C120" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="D120" s="3">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A121" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C121" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="D121" s="3">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A122" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C122" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="D122" s="3">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A123" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C123" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="D123" s="3">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A124" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C124" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="D124" s="3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A125" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C125" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="D125" s="3">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A126" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C126" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="D126" s="3">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A127" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C127" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="D127" s="3">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A128" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C128" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="D128" s="3">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A129" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="B129" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C129" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="D129" s="3">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A130" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C130" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="D130" s="3">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A131" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C131" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="D131" s="3">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A132" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="B132" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C132" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="D132" s="3">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A133" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="B133" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C133" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="D133" s="3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A134" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="B134" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C134" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="D134" s="3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A135" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="B135" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C135" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="D135" s="3">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A136" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B136" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C136" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="D136" s="3">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A137" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="B137" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C137" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="D137" s="3">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A138" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="B138" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C138" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="D138" s="3">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A139" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="B139" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C139" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="D139" s="3">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A140" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="B140" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C140" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="D140" s="3">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A141" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="B141" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C141" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="D141" s="3">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A142" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="B142" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C142" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="D142" s="3">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A143" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="B143" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C143" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="D143" s="3">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A144" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="B144" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C144" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="D144" s="3">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A145" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="B145" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C145" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="D145" s="3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A146" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="B146" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C146" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="D146" s="3">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A147" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="B147" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C147" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="D147" s="3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A148" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="B148" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C148" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="D148" s="3">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A149" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="B149" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C149" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="D149" s="3">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A150" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="B150" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C150" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="D150" s="3">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A151" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="B151" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C151" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="D151" s="3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A152" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="B152" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C152" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="D152" s="3">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A153" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="B153" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C153" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="D153" s="3">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A154" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="B154" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C154" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="D154" s="3">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A155" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="B155" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C155" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="D155" s="3">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A156" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="B156" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C156" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="D156" s="3">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A157" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="B157" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C157" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="D157" s="3">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A158" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="B158" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C158" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="D158" s="3">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A159" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="B159" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C159" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="D159" s="3">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A160" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="B160" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C160" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="D160" s="3">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A161" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="B161" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C161" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="D161" s="3">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A162" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="B162" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C162" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="D162" s="3">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A163" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="B163" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C163" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="D163" s="3">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A164" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="B164" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C164" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="D164" s="3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A165" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="B165" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C165" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="D165" s="3">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A166" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="B166" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C166" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="D166" s="3">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A167" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="B167" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C167" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="D167" s="3">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A168" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="B168" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C168" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="D168" s="3">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A169" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="B169" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C169" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="D169" s="3">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A170" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="B170" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C170" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="D170" s="3">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A171" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="B171" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C171" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="D171" s="3">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A172" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="B172" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C172" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="D172" s="3">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A173" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="B173" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C173" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="D173" s="3">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A174" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="B174" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C174" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="D174" s="3">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A175" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="B175" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C175" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="D175" s="3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A176" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="B176" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C176" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="D176" s="3">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A177" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="B177" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C177" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="D177" s="3">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A178" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="B178" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C178" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="D178" s="3">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A179" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="B179" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C179" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="D179" s="3">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A180" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="B180" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C180" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="D180" s="3">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A181" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="B181" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C181" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="D181" s="3">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A182" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="B182" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C182" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="D182" s="3">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A183" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="B183" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C183" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="D183" s="3">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A184" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="B184" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C184" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="D184" s="3">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A185" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="B185" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C185" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="D185" s="3">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A186" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="B186" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C186" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="D186" s="3">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A187" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="B187" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C187" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="D187" s="3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A188" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="B188" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C188" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="D188" s="3">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A189" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="B189" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C189" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="D189" s="3">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A190" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="B190" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C190" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="D190" s="3">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A191" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="B191" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C191" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="D191" s="3">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A192" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="B192" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C192" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="D192" s="3">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A193" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="B193" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C193" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="D193" s="3">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A194" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="B194" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C194" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="D194" s="3">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A195" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="B195" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C195" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="D195" s="3">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A196" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="B196" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C196" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="D196" s="3">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A197" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="B197" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C197" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="D197" s="3">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A198" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="B198" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C198" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="D198" s="3">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A199" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="B199" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C199" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="D199" s="3">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A200" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="B200" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C200" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="D200" s="3">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A201" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="B201" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C201" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="D201" s="3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A202" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="B202" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C202" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="D202" s="3">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A203" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="B203" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C203" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="D203" s="3">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A204" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="B204" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C204" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="D204" s="3">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A205" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="B205" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C205" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="D205" s="3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A206" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="B206" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C206" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="D206" s="3">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A207" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="B207" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C207" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="D207" s="3">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A208" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="B208" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C208" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="D208" s="3">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A209" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="B209" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C209" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="D209" s="3">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A210" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="B210" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C210" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="D210" s="3">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A211" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="B211" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C211" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="D211" s="3">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A212" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B212" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C212" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="D212" s="3">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A213" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B213" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C213" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="D213" s="3">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A214" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="B214" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C214" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="D214" s="3">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A215" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="B215" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C215" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="D215" s="3">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A216" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="B216" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C216" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="D216" s="3">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A217" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="B217" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C217" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="D217" s="3">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A218" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="B218" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C218" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="D218" s="3">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A219" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="B219" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C219" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="D219" s="3">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A220" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="B220" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C220" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D220" s="3">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A221" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="B221" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C221" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="D221" s="3">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A222" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="B222" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C222" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="D222" s="3">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A223" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="B223" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C223" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="D223" s="3">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A224" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="B224" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C224" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="D224" s="3">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A225" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="B225" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C225" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="D225" s="3">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A226" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="B226" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C226" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="D226" s="3">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A227" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="B227" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C227" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="D227" s="3">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A228" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="B228" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C228" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="D228" s="3">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A229" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="B229" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C229" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D229" s="3">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A230" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="B230" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C230" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="D230" s="3">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A231" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="B231" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C231" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="D231" s="3">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A232" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="B232" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C232" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="D232" s="3">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A233" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="B233" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C233" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="D233" s="3">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A234" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="B234" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C234" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="D234" s="3">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A235" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="B235" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C235" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="D235" s="3">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A236" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="B236" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C236" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="D236" s="3">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A237" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="B237" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C237" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="D237" s="3">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="238" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A238" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="B238" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C238" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="D238" s="3">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A239" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="B239" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C239" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="D239" s="3">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A240" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="B240" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C240" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="D240" s="3">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="241" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A241" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="B241" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C241" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="D241" s="3">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A242" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="B242" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C242" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="D242" s="3">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="243" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A243" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="B243" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C243" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="D243" s="3">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="244" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A244" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="B244" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C244" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="D244" s="3">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="245" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A245" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="B245" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C245" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="D245" s="3">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="246" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A246" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="B246" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C246" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="D246" s="3">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="247" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A247" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="B247" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C247" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="D247" s="3">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="248" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A248" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="B248" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C248" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="D248" s="3">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="249" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A249" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="B249" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C249" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="D249" s="3">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="250" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A250" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="B250" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C250" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="D250" s="3">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="251" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A251" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="B251" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C251" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="D251" s="3">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="252" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A252" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="B252" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C252" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="D252" s="3">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="253" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A253" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="B253" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C253" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="D253" s="3">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="254" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A254" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="B254" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C254" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="D254" s="3">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="255" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A255" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="B255" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C255" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="D255" s="3">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="256" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A256" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="B256" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C256" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="D256" s="3">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="257" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A257" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="B257" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C257" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="D257" s="3">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="258" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A258" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="B258" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C258" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="D258" s="3">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="259" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A259" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="B259" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C259" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="D259" s="3">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="260" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A260" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="B260" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C260" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="D260" s="3">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="261" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A261" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="B261" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C261" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="D261" s="3">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="262" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A262" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="B262" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C262" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="D262" s="3">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="263" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A263" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="B263" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C263" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="D263" s="3">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="264" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A264" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="B264" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C264" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="D264" s="3">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="265" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A265" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="B265" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C265" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="D265" s="3">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="266" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A266" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="B266" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C266" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="D266" s="3">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="267" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A267" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="B267" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C267" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="D267" s="3">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="268" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A268" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="B268" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C268" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="D268" s="3">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="269" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A269" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="B269" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C269" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="D269" s="3">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="270" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A270" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="B270" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C270" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="D270" s="3">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="271" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A271" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="B271" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C271" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="D271" s="3">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="272" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A272" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="B272" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C272" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="D272" s="3">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="273" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A273" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="B273" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C273" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="D273" s="3">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="274" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A274" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="B274" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C274" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="D274" s="3">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="275" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A275" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="B275" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C275" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="D275" s="3">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="276" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A276" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="B276" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C276" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="D276" s="3">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="277" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A277" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="B277" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C277" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="D277" s="3">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="278" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A278" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="B278" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C278" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="D278" s="3">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="279" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A279" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="B279" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C279" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="D279" s="3">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="280" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A280" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="B280" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C280" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="D280" s="3">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="281" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A281" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="B281" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C281" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="D281" s="3">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="282" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A282" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="B282" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C282" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="D282" s="3">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="283" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A283" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="B283" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C283" s="2" t="s">
+        <v>447</v>
+      </c>
+      <c r="D283" s="3">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="284" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A284" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="B284" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C284" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="D284" s="3">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="285" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A285" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="B285" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C285" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="D285" s="3">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="286" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A286" s="2" t="s">
+        <v>452</v>
+      </c>
+      <c r="B286" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C286" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="D286" s="3">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="287" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A287" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="B287" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C287" s="2" t="s">
+        <v>455</v>
+      </c>
+      <c r="D287" s="3">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="288" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A288" s="2" t="s">
+        <v>456</v>
+      </c>
+      <c r="B288" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C288" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="D288" s="3">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="289" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A289" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B289" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C289" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="D289" s="3">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="290" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A290" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="B290" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C290" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="D290" s="3">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="291" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A291" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="B291" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C291" s="2" t="s">
+        <v>460</v>
+      </c>
+      <c r="D291" s="3">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="292" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A292" s="2" t="s">
+        <v>461</v>
+      </c>
+      <c r="B292" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C292" s="2" t="s">
+        <v>462</v>
+      </c>
+      <c r="D292" s="3">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="293" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A293" s="2" t="s">
+        <v>461</v>
+      </c>
+      <c r="B293" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C293" s="2" t="s">
+        <v>463</v>
+      </c>
+      <c r="D293" s="3">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="294" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A294" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="B294" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C294" s="2" t="s">
+        <v>464</v>
+      </c>
+      <c r="D294" s="3">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="295" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A295" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="B295" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C295" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="D295" s="3">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="296" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A296" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="B296" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C296" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="D296" s="3">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="297" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A297" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="B297" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C297" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="D297" s="3">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="298" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A298" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="B298" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C298" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="D298" s="3">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="299" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A299" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="B299" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C299" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="D299" s="3">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="300" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A300" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="B300" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C300" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="D300" s="3">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="301" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A301" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="B301" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C301" s="2" t="s">
+        <v>472</v>
+      </c>
+      <c r="D301" s="3">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="302" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A302" s="2" t="s">
+        <v>473</v>
+      </c>
+      <c r="B302" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C302" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="D302" s="3">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="303" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A303" s="2" t="s">
+        <v>475</v>
+      </c>
+      <c r="B303" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C303" s="2" t="s">
+        <v>476</v>
+      </c>
+      <c r="D303" s="3">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="304" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A304" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="B304" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C304" s="2" t="s">
+        <v>478</v>
+      </c>
+      <c r="D304" s="3">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="305" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A305" s="2" t="s">
+        <v>479</v>
+      </c>
+      <c r="B305" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C305" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="D305" s="3">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="306" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A306" s="2" t="s">
+        <v>481</v>
+      </c>
+      <c r="B306" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C306" s="2" t="s">
+        <v>482</v>
+      </c>
+      <c r="D306" s="3">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="307" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A307" s="2" t="s">
+        <v>483</v>
+      </c>
+      <c r="B307" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C307" s="2" t="s">
+        <v>484</v>
+      </c>
+      <c r="D307" s="3">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="308" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A308" s="2" t="s">
+        <v>485</v>
+      </c>
+      <c r="B308" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C308" s="2" t="s">
+        <v>486</v>
+      </c>
+      <c r="D308" s="3">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="309" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A309" s="2" t="s">
+        <v>487</v>
+      </c>
+      <c r="B309" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C309" s="2" t="s">
+        <v>488</v>
+      </c>
+      <c r="D309" s="3">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="310" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A310" s="2" t="s">
+        <v>489</v>
+      </c>
+      <c r="B310" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C310" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="D310" s="3">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="311" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A311" s="2" t="s">
+        <v>491</v>
+      </c>
+      <c r="B311" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C311" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="D311" s="3">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="312" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A312" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="B312" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C312" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="D312" s="3">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="313" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A313" s="2" t="s">
+        <v>494</v>
+      </c>
+      <c r="B313" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C313" s="2" t="s">
+        <v>495</v>
+      </c>
+      <c r="D313" s="3">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="314" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A314" s="2" t="s">
+        <v>496</v>
+      </c>
+      <c r="B314" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C314" s="2" t="s">
+        <v>497</v>
+      </c>
+      <c r="D314" s="3">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="315" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A315" s="2" t="s">
+        <v>498</v>
+      </c>
+      <c r="B315" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C315" s="2" t="s">
+        <v>499</v>
+      </c>
+      <c r="D315" s="3">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="316" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A316" s="2" t="s">
+        <v>500</v>
+      </c>
+      <c r="B316" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C316" s="2" t="s">
+        <v>501</v>
+      </c>
+      <c r="D316" s="3">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="317" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A317" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="B317" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C317" s="2" t="s">
+        <v>503</v>
+      </c>
+      <c r="D317" s="3">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="318" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A318" s="2" t="s">
+        <v>504</v>
+      </c>
+      <c r="B318" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C318" s="2" t="s">
+        <v>505</v>
+      </c>
+      <c r="D318" s="3">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="319" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A319" s="2" t="s">
+        <v>506</v>
+      </c>
+      <c r="B319" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C319" s="2" t="s">
+        <v>505</v>
+      </c>
+      <c r="D319" s="3">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="320" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A320" s="2" t="s">
+        <v>507</v>
+      </c>
+      <c r="B320" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C320" s="2" t="s">
+        <v>508</v>
+      </c>
+      <c r="D320" s="3">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="321" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A321" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="B321" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C321" s="2" t="s">
+        <v>510</v>
+      </c>
+      <c r="D321" s="3">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="322" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A322" s="2" t="s">
+        <v>511</v>
+      </c>
+      <c r="B322" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C322" s="2" t="s">
+        <v>505</v>
+      </c>
+      <c r="D322" s="3">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="323" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A323" s="2" t="s">
+        <v>512</v>
+      </c>
+      <c r="B323" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C323" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="D323" s="3">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="324" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A324" s="2" t="s">
+        <v>514</v>
+      </c>
+      <c r="B324" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C324" s="2" t="s">
+        <v>515</v>
+      </c>
+      <c r="D324" s="3">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="325" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A325" s="2" t="s">
+        <v>516</v>
+      </c>
+      <c r="B325" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C325" s="2" t="s">
+        <v>517</v>
+      </c>
+      <c r="D325" s="3">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="326" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A326" s="2" t="s">
+        <v>518</v>
+      </c>
+      <c r="B326" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C326" s="2" t="s">
+        <v>519</v>
+      </c>
+      <c r="D326" s="3">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="327" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A327" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="B327" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C327" s="2" t="s">
+        <v>521</v>
+      </c>
+      <c r="D327" s="3">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="328" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A328" s="2" t="s">
+        <v>522</v>
+      </c>
+      <c r="B328" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C328" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="D328" s="3">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="329" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A329" s="2" t="s">
+        <v>524</v>
+      </c>
+      <c r="B329" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C329" s="2" t="s">
+        <v>525</v>
+      </c>
+      <c r="D329" s="3">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="330" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A330" s="2" t="s">
+        <v>526</v>
+      </c>
+      <c r="B330" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C330" s="2" t="s">
+        <v>505</v>
+      </c>
+      <c r="D330" s="3">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="331" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A331" s="2" t="s">
+        <v>527</v>
+      </c>
+      <c r="B331" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C331" s="2" t="s">
+        <v>528</v>
+      </c>
+      <c r="D331" s="3">
+        <v>330</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D102" r:id="rId1" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1239922" xr:uid="{ED1F3A23-AD3A-4519-B3A6-53D1F8B2A97A}"/>
+    <hyperlink ref="D103" r:id="rId2" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1239923" xr:uid="{F04358A7-B4C1-40A3-8266-B72B273554B8}"/>
+    <hyperlink ref="D104" r:id="rId3" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1239924" xr:uid="{9136D805-A08F-481B-8142-35864F4655B3}"/>
+    <hyperlink ref="D105" r:id="rId4" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1239925" xr:uid="{746AD766-86BF-4B8B-AEC4-98FFF595B18E}"/>
+    <hyperlink ref="D106" r:id="rId5" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1239926" xr:uid="{9CE3DA0A-87EB-46B2-8B4B-2DB1F0FF6E64}"/>
+    <hyperlink ref="D107" r:id="rId6" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1239927" xr:uid="{0CA855B2-049B-455C-B915-908B646B1D49}"/>
+    <hyperlink ref="D108" r:id="rId7" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1239928" xr:uid="{C0CD9B49-8DC9-4992-9566-C8F080A19BC6}"/>
+    <hyperlink ref="D109" r:id="rId8" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1239929" xr:uid="{DD4F9D73-22DE-4F90-B3C1-AE5C3B80406F}"/>
+    <hyperlink ref="D110" r:id="rId9" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1239930" xr:uid="{BDAD5C4E-2875-460E-875E-59452670B3D6}"/>
+    <hyperlink ref="D111" r:id="rId10" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1239931" xr:uid="{1647D183-5D64-4CB4-BB05-CFD682668488}"/>
+    <hyperlink ref="D112" r:id="rId11" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1239932" xr:uid="{B4F86367-3B3B-4322-96F2-2C80DCF23DC5}"/>
+    <hyperlink ref="D113" r:id="rId12" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1239933" xr:uid="{A859490F-A902-4740-8D44-9A4F21286AC0}"/>
+    <hyperlink ref="D114" r:id="rId13" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1239934" xr:uid="{B7BC8B0D-2A19-409A-BDCD-562BFD248F01}"/>
+    <hyperlink ref="D115" r:id="rId14" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1239935" xr:uid="{C2ABDEA2-C3AD-4767-807D-4DCDF26D5E46}"/>
+    <hyperlink ref="D116" r:id="rId15" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1239936" xr:uid="{4C842806-C20A-42B9-97B2-C37B228AFF08}"/>
+    <hyperlink ref="D117" r:id="rId16" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1239937" xr:uid="{BC289388-0F26-44FE-9E34-18D0C258CEE3}"/>
+    <hyperlink ref="D118" r:id="rId17" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1239938" xr:uid="{FB51FA97-F903-4D43-92CC-BD5956B5E9B7}"/>
+    <hyperlink ref="D119" r:id="rId18" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1239939" xr:uid="{41B134C6-26C9-420C-8817-235755D7D0BA}"/>
+    <hyperlink ref="D120" r:id="rId19" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1239940" xr:uid="{2C7F26F2-5BA7-4646-A568-F74E4CD8A0D9}"/>
+    <hyperlink ref="D121" r:id="rId20" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1239941" xr:uid="{564BAB39-E0B2-4B5F-87D8-17DED2ACB563}"/>
+    <hyperlink ref="D122" r:id="rId21" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1239942" xr:uid="{38320D14-1C47-4F17-88C1-F36409DAB41B}"/>
+    <hyperlink ref="D123" r:id="rId22" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1239943" xr:uid="{77006249-E184-48FB-8C0E-5B8B9AD366DC}"/>
+    <hyperlink ref="D124" r:id="rId23" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1239944" xr:uid="{1F217288-E5E0-4A5A-9779-C39B146BDA00}"/>
+    <hyperlink ref="D125" r:id="rId24" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1239945" xr:uid="{5C41AFB5-1E8A-4793-AA89-8959583FA525}"/>
+    <hyperlink ref="D126" r:id="rId25" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1239946" xr:uid="{E271B362-22BD-4284-A098-1882D9C70516}"/>
+    <hyperlink ref="D127" r:id="rId26" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1239947" xr:uid="{9124368F-7D5D-488B-A67C-6F7EA6618D55}"/>
+    <hyperlink ref="D128" r:id="rId27" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1239948" xr:uid="{C567B1B8-2933-426E-B3C9-E6CD39259171}"/>
+    <hyperlink ref="D129" r:id="rId28" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1239949" xr:uid="{CDC6A8AF-CB21-4072-9722-F4998CA0700F}"/>
+    <hyperlink ref="D130" r:id="rId29" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1239950" xr:uid="{5425D166-7319-43AC-98F4-0C10D06775AD}"/>
+    <hyperlink ref="D131" r:id="rId30" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1239951" xr:uid="{C37B91B5-D341-48E0-A313-FB0D5E5DBFF2}"/>
+    <hyperlink ref="D132" r:id="rId31" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1239952" xr:uid="{3D5AB34D-8A26-4835-911C-FDA5CFF256DB}"/>
+    <hyperlink ref="D133" r:id="rId32" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1239953" xr:uid="{5F4FB28B-B750-4B8F-8398-33B3FB4CCDA5}"/>
+    <hyperlink ref="D134" r:id="rId33" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1239954" xr:uid="{E8F0576E-6401-43C6-9047-AE2D69285FE6}"/>
+    <hyperlink ref="D135" r:id="rId34" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1239955" xr:uid="{7CD6C388-C905-4B7A-9C95-32E688234D8A}"/>
+    <hyperlink ref="D136" r:id="rId35" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1239956" xr:uid="{73F9891D-0BE9-423A-90B6-4DDCF35548E3}"/>
+    <hyperlink ref="D137" r:id="rId36" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1239957" xr:uid="{9E0C0019-CACC-49B6-889F-AC57A667FB41}"/>
+    <hyperlink ref="D138" r:id="rId37" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1239958" xr:uid="{E99196F3-3ABB-40FA-9CCC-E3B9E4723422}"/>
+    <hyperlink ref="D139" r:id="rId38" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1239959" xr:uid="{459C8B82-BF7D-4486-BCEF-6C09BBE9AF30}"/>
+    <hyperlink ref="D140" r:id="rId39" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1239960" xr:uid="{25A93115-9106-41DE-94EA-E32F6BE053E3}"/>
+    <hyperlink ref="D141" r:id="rId40" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1239961" xr:uid="{40C17756-DEEE-4FAD-AAF7-64FBCFAFEE5D}"/>
+    <hyperlink ref="D142" r:id="rId41" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1239962" xr:uid="{6A576E9A-423E-4DD0-B168-ADED295E514F}"/>
+    <hyperlink ref="D143" r:id="rId42" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1239963" xr:uid="{154E76C5-FAE1-459A-BF07-DAEE06C536E0}"/>
+    <hyperlink ref="D144" r:id="rId43" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1239964" xr:uid="{98C28164-16DA-4504-BC77-B99699F983EA}"/>
+    <hyperlink ref="D145" r:id="rId44" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1239965" xr:uid="{0B94B9EA-0817-4920-9AB6-9D32883F0E2F}"/>
+    <hyperlink ref="D146" r:id="rId45" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1239966" xr:uid="{72BCD13B-F6CA-40B6-9AB6-9DBBB77007D6}"/>
+    <hyperlink ref="D147" r:id="rId46" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1239967" xr:uid="{A923097F-5B03-4490-9951-C65B2BDC06E1}"/>
+    <hyperlink ref="D148" r:id="rId47" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1239968" xr:uid="{1F681E69-C55A-4C05-B020-B8CE100D651A}"/>
+    <hyperlink ref="D149" r:id="rId48" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1239969" xr:uid="{AB10B70E-0E08-485F-BD02-812EACB5DE2E}"/>
+    <hyperlink ref="D150" r:id="rId49" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1239970" xr:uid="{4BAAEC5C-7DC7-4172-A326-C19D2115522D}"/>
+    <hyperlink ref="D151" r:id="rId50" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1239971" xr:uid="{F00E8914-75BA-4DF6-B3E3-7BB5257E6C89}"/>
+    <hyperlink ref="D152" r:id="rId51" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1239972" xr:uid="{67AB1182-4700-4AD3-A4A5-55FD4C8D5A67}"/>
+    <hyperlink ref="D153" r:id="rId52" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1239973" xr:uid="{BBDC966E-2E64-44E6-9364-D3F737383582}"/>
+    <hyperlink ref="D154" r:id="rId53" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1239974" xr:uid="{74925390-4C73-43EB-B43F-82CF327B6D2F}"/>
+    <hyperlink ref="D155" r:id="rId54" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1239975" xr:uid="{6DA40927-E97D-4E3B-BAAC-7888EDC0B45E}"/>
+    <hyperlink ref="D156" r:id="rId55" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1239976" xr:uid="{A495CD22-E42E-4A1E-9CDF-7F4F90F9C10D}"/>
+    <hyperlink ref="D157" r:id="rId56" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1239977" xr:uid="{D4120379-BC4E-4764-86D0-EA20080A970A}"/>
+    <hyperlink ref="D158" r:id="rId57" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1239978" xr:uid="{7357E4BD-2EC6-4960-9BE7-93ABA045B757}"/>
+    <hyperlink ref="D159" r:id="rId58" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1239979" xr:uid="{D3672BE2-ADCA-4AC7-A936-24C3659040B7}"/>
+    <hyperlink ref="D160" r:id="rId59" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1239980" xr:uid="{33E0E898-3A97-4EBA-A6FE-0920E27147B8}"/>
+    <hyperlink ref="D161" r:id="rId60" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1239981" xr:uid="{8AB252A5-8F0F-4E52-8CE3-55479CB7F58D}"/>
+    <hyperlink ref="D162" r:id="rId61" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1239982" xr:uid="{EF067E10-46A9-4989-B228-0B03B11B60C6}"/>
+    <hyperlink ref="D163" r:id="rId62" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1239983" xr:uid="{140FC653-2C46-42B9-8C7A-7625E27E91D1}"/>
+    <hyperlink ref="D164" r:id="rId63" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1239984" xr:uid="{7BF4B7DF-BC1E-4EBE-8C98-7FD7456240F9}"/>
+    <hyperlink ref="D165" r:id="rId64" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1239985" xr:uid="{C5BE6E8C-CCC8-45C5-A2D8-D4F2D38EBA33}"/>
+    <hyperlink ref="D166" r:id="rId65" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1239986" xr:uid="{E16B63F5-4B34-47FB-B572-B7E36226047A}"/>
+    <hyperlink ref="D167" r:id="rId66" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1239987" xr:uid="{A2341A36-C38C-4710-8875-BF906A70643F}"/>
+    <hyperlink ref="D168" r:id="rId67" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1239988" xr:uid="{C85FC8E3-7FE8-45E1-AC39-BFB634F45E66}"/>
+    <hyperlink ref="D169" r:id="rId68" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1239989" xr:uid="{BDC45D51-5824-4FB8-B9AD-CF117F2ACBE9}"/>
+    <hyperlink ref="D170" r:id="rId69" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1239990" xr:uid="{4FCCBCB9-AB67-4CC8-B06B-E3A380233A47}"/>
+    <hyperlink ref="D171" r:id="rId70" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1239991" xr:uid="{92191E9B-F368-42D1-A138-1F6E606653A4}"/>
+    <hyperlink ref="D172" r:id="rId71" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1239992" xr:uid="{3AD2CDE3-A5FE-47FE-B5AE-8681E1BCC3F4}"/>
+    <hyperlink ref="D173" r:id="rId72" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1239993" xr:uid="{0473D649-850F-4F0E-9F42-66F5AAE946F2}"/>
+    <hyperlink ref="D174" r:id="rId73" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1239994" xr:uid="{417BF8D3-6DDC-4DC5-BF8B-EB6B07CD1F4D}"/>
+    <hyperlink ref="D175" r:id="rId74" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1239995" xr:uid="{D09C90CD-1740-4B5E-A489-38A6E6148701}"/>
+    <hyperlink ref="D176" r:id="rId75" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1239996" xr:uid="{3259C0D1-E241-4619-B7F9-C84A5528C8BA}"/>
+    <hyperlink ref="D177" r:id="rId76" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1239997" xr:uid="{1DF50E09-02CC-48E3-AD7C-5C0FEF990D87}"/>
+    <hyperlink ref="D178" r:id="rId77" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1239998" xr:uid="{FF8A6708-2DAD-4076-94A2-3D0262495F52}"/>
+    <hyperlink ref="D179" r:id="rId78" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1239999" xr:uid="{BD4F791D-6A78-4557-ACDF-705E6155BD1D}"/>
+    <hyperlink ref="D180" r:id="rId79" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240000" xr:uid="{26F11EB1-D301-4DFA-97FE-503730F8D6D2}"/>
+    <hyperlink ref="D181" r:id="rId80" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240001" xr:uid="{628A0814-C566-4573-AA26-849E29FBA0AA}"/>
+    <hyperlink ref="D182" r:id="rId81" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240002" xr:uid="{A1D81DC9-C179-4810-9E65-B447B7B33928}"/>
+    <hyperlink ref="D183" r:id="rId82" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240003" xr:uid="{19C93FDE-8194-444A-9C49-874371D4C0F8}"/>
+    <hyperlink ref="D184" r:id="rId83" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240004" xr:uid="{71908C7F-2183-4E8E-800D-5A98BAF24A02}"/>
+    <hyperlink ref="D185" r:id="rId84" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240005" xr:uid="{7D37C565-515F-4146-97CE-DAB44318D9B9}"/>
+    <hyperlink ref="D186" r:id="rId85" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240006" xr:uid="{B04E491E-9410-4FF2-ACEB-3C90D0068090}"/>
+    <hyperlink ref="D187" r:id="rId86" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240007" xr:uid="{A5FE8679-D45F-416A-AF8E-6AD00F208486}"/>
+    <hyperlink ref="D188" r:id="rId87" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240008" xr:uid="{F7F4CD10-322F-4D0A-A734-E6FF2E7DD0F5}"/>
+    <hyperlink ref="D189" r:id="rId88" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240009" xr:uid="{332D01DE-7129-4027-872B-9CD4E080B8A2}"/>
+    <hyperlink ref="D190" r:id="rId89" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240010" xr:uid="{3E1AC378-2B4A-42DB-8BB7-47AA71BD7B4E}"/>
+    <hyperlink ref="D191" r:id="rId90" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240011" xr:uid="{78554897-6ED8-4F17-9F0F-1A1C3A7EFAFE}"/>
+    <hyperlink ref="D192" r:id="rId91" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240012" xr:uid="{E2EB2118-9D1D-4FC8-A5D9-CBC0D310934F}"/>
+    <hyperlink ref="D193" r:id="rId92" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240013" xr:uid="{AC7273C2-2028-44F2-8CBB-5DEDD69907C0}"/>
+    <hyperlink ref="D194" r:id="rId93" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240014" xr:uid="{F69CB5B0-D2F4-419B-AD30-F21ACF8301F5}"/>
+    <hyperlink ref="D195" r:id="rId94" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240015" xr:uid="{AA05C23D-7568-415C-8729-731C86ECA199}"/>
+    <hyperlink ref="D196" r:id="rId95" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240016" xr:uid="{9B9CC434-ADD6-4543-9E34-213FEBFF1247}"/>
+    <hyperlink ref="D197" r:id="rId96" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240017" xr:uid="{1B7FC30B-4157-4CF2-961C-4A7F36BAA93E}"/>
+    <hyperlink ref="D198" r:id="rId97" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240018" xr:uid="{4577AC5A-58FE-45D6-AAB8-092C10BEECAC}"/>
+    <hyperlink ref="D199" r:id="rId98" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240019" xr:uid="{3F6CEC98-4F95-48DF-A221-A81B27CF61F1}"/>
+    <hyperlink ref="D200" r:id="rId99" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240020" xr:uid="{98949832-87AA-4F28-8DFE-74AED4D256CB}"/>
+    <hyperlink ref="D201" r:id="rId100" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240021" xr:uid="{EBED1656-AE59-4CE8-81AA-9671C4CA31E9}"/>
+    <hyperlink ref="D202" r:id="rId101" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240022" xr:uid="{142C79D2-2045-4E0E-8C50-6DDCE752F139}"/>
+    <hyperlink ref="D203" r:id="rId102" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240023" xr:uid="{15328037-9886-49CC-A9FA-D070CB895B2A}"/>
+    <hyperlink ref="D204" r:id="rId103" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240024" xr:uid="{6C1F8625-D08C-4F5F-95F3-9E0F7FCB26BC}"/>
+    <hyperlink ref="D205" r:id="rId104" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240025" xr:uid="{C1C1A4B0-856F-46DB-A8A5-5C70C4F55C18}"/>
+    <hyperlink ref="D206" r:id="rId105" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240026" xr:uid="{09D2AF6C-2A5D-44FD-A3EC-EAD206B05F37}"/>
+    <hyperlink ref="D207" r:id="rId106" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240027" xr:uid="{4C6D45E1-5D1D-4073-BF59-C99CB57B7202}"/>
+    <hyperlink ref="D208" r:id="rId107" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240028" xr:uid="{C9DDFD93-E966-464C-8898-E74C8B4A1949}"/>
+    <hyperlink ref="D209" r:id="rId108" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240029" xr:uid="{CF8A8E44-C7FE-4E1D-87C1-3C342E2649F4}"/>
+    <hyperlink ref="D210" r:id="rId109" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240030" xr:uid="{904694FE-61C1-4AF5-80A4-09456B2DDCF0}"/>
+    <hyperlink ref="D211" r:id="rId110" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240031" xr:uid="{247EC425-8213-4ABB-BB56-5E75474DFC8F}"/>
+    <hyperlink ref="D212" r:id="rId111" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240032" xr:uid="{D9BB95D1-9626-4597-BC3D-D6FB3569D10E}"/>
+    <hyperlink ref="D213" r:id="rId112" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240033" xr:uid="{75FFEB3D-BB75-49DB-B409-503E64EF5B1B}"/>
+    <hyperlink ref="D214" r:id="rId113" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240034" xr:uid="{325C45CF-D774-4868-85CB-85E41F612528}"/>
+    <hyperlink ref="D215" r:id="rId114" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240035" xr:uid="{75BE5335-3D16-44AA-BFB1-C0438EBE248F}"/>
+    <hyperlink ref="D216" r:id="rId115" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240036" xr:uid="{31F9BE85-0E07-4D6C-91DD-C4D390FB0BE7}"/>
+    <hyperlink ref="D217" r:id="rId116" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240037" xr:uid="{994924C2-386A-49CD-B692-31454251D220}"/>
+    <hyperlink ref="D218" r:id="rId117" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240038" xr:uid="{A3FCD3A4-497C-430B-B44C-7F002CE62D0F}"/>
+    <hyperlink ref="D219" r:id="rId118" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240039" xr:uid="{2A0E868B-A943-4F8D-AB57-A1F2090F541A}"/>
+    <hyperlink ref="D220" r:id="rId119" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240040" xr:uid="{F28D0BC4-35BA-4068-9BD1-8FA2E4C03C31}"/>
+    <hyperlink ref="D221" r:id="rId120" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240041" xr:uid="{7B44B29B-18F2-41F2-9B09-D7F52732CC6F}"/>
+    <hyperlink ref="D222" r:id="rId121" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240042" xr:uid="{41587B67-9185-4685-86CB-9186E1ABDCAA}"/>
+    <hyperlink ref="D223" r:id="rId122" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240043" xr:uid="{ED8BD70A-F683-46FA-9464-241268647023}"/>
+    <hyperlink ref="D224" r:id="rId123" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240044" xr:uid="{5885EFB1-B4ED-4CB3-8CF0-AC53A80684CB}"/>
+    <hyperlink ref="D225" r:id="rId124" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240045" xr:uid="{7B6A9033-43CA-4E7B-932A-5BFCFF2D4673}"/>
+    <hyperlink ref="D226" r:id="rId125" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240046" xr:uid="{2A10A66A-BE42-4ACE-9B61-BAEC343B3AD7}"/>
+    <hyperlink ref="D227" r:id="rId126" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240047" xr:uid="{1E75BA57-183D-4F69-9646-D491C64D5597}"/>
+    <hyperlink ref="D228" r:id="rId127" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240048" xr:uid="{D38C9F17-4461-4E34-950E-1CDEED7F3D4A}"/>
+    <hyperlink ref="D229" r:id="rId128" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240049" xr:uid="{3956B86A-5C2B-4088-82C3-696D832E9F16}"/>
+    <hyperlink ref="D230" r:id="rId129" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240050" xr:uid="{EA564A71-E0DE-4585-AA2E-88930C943F84}"/>
+    <hyperlink ref="D231" r:id="rId130" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240051" xr:uid="{47F8E8E2-BB77-4A64-BF64-50E17DA77DEA}"/>
+    <hyperlink ref="D232" r:id="rId131" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240052" xr:uid="{CDAED21E-2D02-45C3-B9A3-1FBD21BD62D6}"/>
+    <hyperlink ref="D233" r:id="rId132" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240053" xr:uid="{DA719C85-F88E-48FF-A551-2CE8CF796E2A}"/>
+    <hyperlink ref="D234" r:id="rId133" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240054" xr:uid="{8820C1BF-90A2-4258-AE32-BDC8CC8F93BC}"/>
+    <hyperlink ref="D235" r:id="rId134" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240055" xr:uid="{4E8732BE-9D61-4F75-8DEE-1F9B4B34A641}"/>
+    <hyperlink ref="D236" r:id="rId135" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240056" xr:uid="{236F74E8-9104-467D-AD1D-6B64FAC41D3E}"/>
+    <hyperlink ref="D237" r:id="rId136" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240057" xr:uid="{4CA9CD8E-159C-4ED5-9B2B-4A0A6B9BAF0B}"/>
+    <hyperlink ref="D238" r:id="rId137" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240058" xr:uid="{EC0B29BF-58CA-4145-A515-43248F4152FB}"/>
+    <hyperlink ref="D239" r:id="rId138" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240059" xr:uid="{511F4EC7-761E-47BE-A6D5-CD95B372D9B1}"/>
+    <hyperlink ref="D240" r:id="rId139" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240060" xr:uid="{0DBF706E-EA0B-48A3-81FF-7EBE2792D867}"/>
+    <hyperlink ref="D241" r:id="rId140" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240061" xr:uid="{5F368BB5-9B7A-4C89-878B-A6847CACC17D}"/>
+    <hyperlink ref="D242" r:id="rId141" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240062" xr:uid="{9634E9F3-2FD7-4535-9F47-C4BF6C706CF7}"/>
+    <hyperlink ref="D243" r:id="rId142" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240063" xr:uid="{4FBCE3B6-72B1-470B-B8DB-929C3ED272DA}"/>
+    <hyperlink ref="D244" r:id="rId143" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240064" xr:uid="{14822083-6CEC-4C16-A3BD-7F0B88FD4E8D}"/>
+    <hyperlink ref="D245" r:id="rId144" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240065" xr:uid="{7E007441-08CD-4AE4-8575-0453E792F018}"/>
+    <hyperlink ref="D246" r:id="rId145" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240066" xr:uid="{C03A7653-3E43-4319-941B-DA1830AA37B3}"/>
+    <hyperlink ref="D247" r:id="rId146" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240067" xr:uid="{BFE0E71F-CF4F-4C81-AB94-DC17FDBB40E9}"/>
+    <hyperlink ref="D248" r:id="rId147" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240068" xr:uid="{DAA4A090-98B4-461E-96B6-10AC33244796}"/>
+    <hyperlink ref="D249" r:id="rId148" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240069" xr:uid="{1131E0B6-9544-44AD-AF35-0ACB564A7925}"/>
+    <hyperlink ref="D250" r:id="rId149" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240070" xr:uid="{77D95A6E-699E-4290-99DD-DE33CBF21703}"/>
+    <hyperlink ref="D251" r:id="rId150" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240071" xr:uid="{F68B59AA-1F90-410D-8FE0-0D891B23818C}"/>
+    <hyperlink ref="D252" r:id="rId151" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240072" xr:uid="{B0630163-5F65-4198-AB57-F731DF744E17}"/>
+    <hyperlink ref="D253" r:id="rId152" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240073" xr:uid="{5AF84F0F-A324-4A76-9E4C-B4E6E02619A1}"/>
+    <hyperlink ref="D254" r:id="rId153" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240074" xr:uid="{BAB1C1D5-A182-4653-B5E2-DA2258A502C9}"/>
+    <hyperlink ref="D255" r:id="rId154" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240075" xr:uid="{9E7F47F7-618C-4707-9CA5-9954BA7FF8DC}"/>
+    <hyperlink ref="D256" r:id="rId155" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240076" xr:uid="{BF3CAE7F-F652-4574-8E43-A86285B3C25D}"/>
+    <hyperlink ref="D257" r:id="rId156" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240077" xr:uid="{3FBCA90C-9CE1-4420-8D21-D27C8BECCBC4}"/>
+    <hyperlink ref="D258" r:id="rId157" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240078" xr:uid="{FF26533F-FCE2-402C-B772-BAC4E1DB060D}"/>
+    <hyperlink ref="D259" r:id="rId158" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240079" xr:uid="{E7E547B2-2C8D-47AE-AB78-AD8C4573A738}"/>
+    <hyperlink ref="D260" r:id="rId159" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240080" xr:uid="{AD5E02EB-DF94-4FED-AB14-31ECB16CE961}"/>
+    <hyperlink ref="D261" r:id="rId160" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240081" xr:uid="{F603CD2D-C240-44B2-99D3-130CBFC75B50}"/>
+    <hyperlink ref="D262" r:id="rId161" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240082" xr:uid="{8B13BF79-5FE5-4C39-BC3A-D484A9E1D587}"/>
+    <hyperlink ref="D263" r:id="rId162" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240083" xr:uid="{B3B608BD-970B-427C-9774-A27E635B4EEC}"/>
+    <hyperlink ref="D264" r:id="rId163" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240084" xr:uid="{A4F9C6B8-D383-43A6-B9F9-DDD231721DEC}"/>
+    <hyperlink ref="D265" r:id="rId164" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240085" xr:uid="{418B67A9-71FA-4C65-AB88-96E6B0E2B85A}"/>
+    <hyperlink ref="D266" r:id="rId165" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240086" xr:uid="{44023C71-905D-42AB-BD08-8362925CF8EC}"/>
+    <hyperlink ref="D267" r:id="rId166" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240087" xr:uid="{6C9B133C-BC95-436A-A6E3-DA02E0874CFE}"/>
+    <hyperlink ref="D268" r:id="rId167" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240088" xr:uid="{F129086E-9CB1-45F0-8D37-7112AEC0030C}"/>
+    <hyperlink ref="D269" r:id="rId168" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240089" xr:uid="{27319A40-1A78-4A5F-880B-AD715BD41CC0}"/>
+    <hyperlink ref="D270" r:id="rId169" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240090" xr:uid="{C4259C8E-0388-4869-8449-8B1294B56F8F}"/>
+    <hyperlink ref="D271" r:id="rId170" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240091" xr:uid="{4360DC4F-FB9E-418A-B3FA-E82D9D9DD268}"/>
+    <hyperlink ref="D272" r:id="rId171" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240092" xr:uid="{957FF92D-5628-4E0F-976B-F5F52A4B5BC4}"/>
+    <hyperlink ref="D273" r:id="rId172" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240093" xr:uid="{C861A189-F01A-4DEC-A224-F4AE70168E8B}"/>
+    <hyperlink ref="D274" r:id="rId173" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240094" xr:uid="{694ED214-D988-47A7-9EFD-CD7EDDDCA1B2}"/>
+    <hyperlink ref="D275" r:id="rId174" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240095" xr:uid="{41D7C3C9-9D56-4894-975D-7BFA6162C7CA}"/>
+    <hyperlink ref="D276" r:id="rId175" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240096" xr:uid="{1FF8959F-2F25-49C8-A7CF-76FD7952C17D}"/>
+    <hyperlink ref="D277" r:id="rId176" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240097" xr:uid="{D7FC961F-D42D-4207-A019-07E7D40CCB32}"/>
+    <hyperlink ref="D278" r:id="rId177" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240098" xr:uid="{EBC58ED7-CB3E-44EA-B2EA-F3CE8586BAE3}"/>
+    <hyperlink ref="D279" r:id="rId178" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240099" xr:uid="{C86B888D-0F8B-4DFC-9647-730DEA8247DE}"/>
+    <hyperlink ref="D280" r:id="rId179" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240100" xr:uid="{52034DA1-3BA8-403E-ACDE-ACADFD1FF4AF}"/>
+    <hyperlink ref="D281" r:id="rId180" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240101" xr:uid="{1519D457-C13E-424B-80B7-B10412CA33D2}"/>
+    <hyperlink ref="D282" r:id="rId181" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240102" xr:uid="{5C47D118-EFC9-4747-B003-F9A4B19AA61F}"/>
+    <hyperlink ref="D283" r:id="rId182" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240103" xr:uid="{781666BD-81DC-4E2C-857C-69F57CBB05F8}"/>
+    <hyperlink ref="D284" r:id="rId183" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240104" xr:uid="{02063554-ABD0-4A9F-9043-91D786B8276B}"/>
+    <hyperlink ref="D285" r:id="rId184" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240105" xr:uid="{A069BC97-90AD-4952-AF37-ED26A3F4D508}"/>
+    <hyperlink ref="D286" r:id="rId185" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240106" xr:uid="{CC4C0803-2913-464A-B959-4E58CCA007A4}"/>
+    <hyperlink ref="D287" r:id="rId186" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1240107" xr:uid="{8C40978E-E83D-40DC-90EA-40E4333991BF}"/>
+    <hyperlink ref="D288" r:id="rId187" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1269366" xr:uid="{928F0B87-E660-462B-B96F-3C10DB83D344}"/>
+    <hyperlink ref="D289" r:id="rId188" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1269371" xr:uid="{A2179044-3E29-467C-BBDF-08C4BAE33C47}"/>
+    <hyperlink ref="D290" r:id="rId189" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1269373" xr:uid="{798C63C7-BB8C-4535-9644-3705FEEDF390}"/>
+    <hyperlink ref="D291" r:id="rId190" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1269375" xr:uid="{295CC231-53E2-442E-B97C-04D9ABBD7CAF}"/>
+    <hyperlink ref="D292" r:id="rId191" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1269377" xr:uid="{0B3E59C2-EE32-41CA-9E4E-7D12B753DF01}"/>
+    <hyperlink ref="D293" r:id="rId192" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1269391" xr:uid="{1CF3468A-9118-4E5F-9D67-35099AFED3D6}"/>
+    <hyperlink ref="D294" r:id="rId193" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1269393" xr:uid="{940D63F5-7EE9-47C8-8A29-D45E41AB5692}"/>
+    <hyperlink ref="D295" r:id="rId194" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1269396" xr:uid="{C1838085-A9CB-4945-82C3-1CE92E4213E4}"/>
+    <hyperlink ref="D296" r:id="rId195" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1269398" xr:uid="{862D678F-6827-4619-8FFA-30E233DBDCDB}"/>
+    <hyperlink ref="D297" r:id="rId196" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1269400" xr:uid="{C6129114-48AC-41D3-A53D-78CD863B1696}"/>
+    <hyperlink ref="D298" r:id="rId197" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1269403" xr:uid="{627C10C7-8845-4A21-8BC0-CFAF8A442A05}"/>
+    <hyperlink ref="D299" r:id="rId198" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1269409" xr:uid="{6ABADF52-0910-4E13-B7B1-FB1E153028CE}"/>
+    <hyperlink ref="D300" r:id="rId199" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1269411" xr:uid="{51DE493B-C616-4ECB-AA98-EB0314FF2806}"/>
+    <hyperlink ref="D301" r:id="rId200" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1269413" xr:uid="{D74257FF-BA46-423D-93F3-7E6DBE17D3F7}"/>
+    <hyperlink ref="D302" r:id="rId201" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1269418" xr:uid="{51596FFA-1AEE-4566-8940-91A190FC767D}"/>
+    <hyperlink ref="D303" r:id="rId202" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1267703" xr:uid="{7E04FD8A-E68E-40BB-9633-496D0FF4AA99}"/>
+    <hyperlink ref="D304" r:id="rId203" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1267704" xr:uid="{392EA8FC-1EA3-414F-B1E8-63FF69A683C2}"/>
+    <hyperlink ref="D305" r:id="rId204" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1267705" xr:uid="{F33FD946-2B01-4ABD-824F-C14A1135800D}"/>
+    <hyperlink ref="D306" r:id="rId205" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1267706" xr:uid="{F4E8B470-495F-4D19-B447-667C25C8A2A5}"/>
+    <hyperlink ref="D307" r:id="rId206" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1267707" xr:uid="{CF73B54A-23D9-4247-B998-2C8C11C075BA}"/>
+    <hyperlink ref="D308" r:id="rId207" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1267708" xr:uid="{925E0BF0-2166-4AE7-88BC-AFFD6C07BC2D}"/>
+    <hyperlink ref="D309" r:id="rId208" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1267709" xr:uid="{C45099C8-EC64-4473-88A4-8BA29AE9E8DC}"/>
+    <hyperlink ref="D310" r:id="rId209" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1267711" xr:uid="{0393538D-F003-4FDD-BDB8-D68DCD961582}"/>
+    <hyperlink ref="D311" r:id="rId210" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1267712" xr:uid="{4ED17279-A0F7-4613-B81A-E12F37800EE8}"/>
+    <hyperlink ref="D312" r:id="rId211" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1267713" xr:uid="{9BA12704-69AB-42FA-AFEC-F3FE006B18CB}"/>
+    <hyperlink ref="D313" r:id="rId212" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1267714" xr:uid="{9DE87305-3827-4D0C-B921-A8D62498ED1D}"/>
+    <hyperlink ref="D314" r:id="rId213" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1267715" xr:uid="{E50E0DA3-2854-4B8A-AA7A-8C78E8C901CD}"/>
+    <hyperlink ref="D315" r:id="rId214" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1267716" xr:uid="{FC4CB476-D3B5-4FD2-8F4B-1B7243BA52DF}"/>
+    <hyperlink ref="D316" r:id="rId215" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1267717" xr:uid="{F3FCF105-C4D6-49D4-802F-CE7B0E85C99B}"/>
+    <hyperlink ref="D317" r:id="rId216" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1267718" xr:uid="{05674234-4008-41BF-BDDD-8BAA8D4EE657}"/>
+    <hyperlink ref="D318" r:id="rId217" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1267719" xr:uid="{3228F7E1-D07A-4ACC-94D3-391829DB79EC}"/>
+    <hyperlink ref="D319" r:id="rId218" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1267720" xr:uid="{4728ED2A-6910-4ADF-9F5D-57DED763EB26}"/>
+    <hyperlink ref="D320" r:id="rId219" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1267721" xr:uid="{EF075033-4C3A-4B43-92CD-4867D62E57A1}"/>
+    <hyperlink ref="D321" r:id="rId220" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1267722" xr:uid="{6AB75D3F-F267-4D11-9B4D-1B81EFCB208B}"/>
+    <hyperlink ref="D322" r:id="rId221" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1267723" xr:uid="{2E678811-8FD9-43C7-BD5C-A14169F6BB15}"/>
+    <hyperlink ref="D323" r:id="rId222" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1267724" xr:uid="{4E9DFBCE-BF8A-43D3-A30C-7A4268091BC5}"/>
+    <hyperlink ref="D324" r:id="rId223" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1267725" xr:uid="{000B03CC-0140-422C-8676-AFEDB94BBFF5}"/>
+    <hyperlink ref="D325" r:id="rId224" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1267726" xr:uid="{D0D2A1AC-85C1-4843-B910-6D04551263FA}"/>
+    <hyperlink ref="D326" r:id="rId225" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1267727" xr:uid="{7DB7DEF7-FE1B-4D6A-9714-56C6B79649E0}"/>
+    <hyperlink ref="D327" r:id="rId226" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1267728" xr:uid="{70EE2ED1-F67E-4747-90D8-E4338E566CA3}"/>
+    <hyperlink ref="D328" r:id="rId227" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1267730" xr:uid="{33B8A0DC-890C-40B5-9998-83EA75150F9F}"/>
+    <hyperlink ref="D329" r:id="rId228" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1267731" xr:uid="{404484F8-91CB-4B64-8750-77E3994E3D43}"/>
+    <hyperlink ref="D330" r:id="rId229" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1267732" xr:uid="{DABE0AAC-CA40-49E8-A610-B5EDA6DAB8B5}"/>
+    <hyperlink ref="D331" r:id="rId230" display="https://samorzad2024.pkw.gov.pl/samorzad2024/pl/obkw/1269762" xr:uid="{8945F771-CBE3-4B1E-B528-0AA48210A81E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>